<commit_message>
Update Schedule: move TDD to KW19
</commit_message>
<xml_diff>
--- a/planung_pm.xlsx
+++ b/planung_pm.xlsx
@@ -5,9 +5,9 @@
   <sheets>
     <sheet state="hidden" name="Themen" sheetId="1" r:id="rId4"/>
     <sheet state="hidden" name="Wochenüberblick (alt Formeln)" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Wochenüberblick (alt VL Mo)" sheetId="3" r:id="rId6"/>
+    <sheet state="hidden" name="Wochenüberblick (alt VL Mo)" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="V1 (neu VL Fr)" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="V2 (neu VL Fr)" sheetId="5" r:id="rId8"/>
+    <sheet state="hidden" name="V2 (neu VL Fr)" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="241">
   <si>
     <t>Thema</t>
   </si>
@@ -626,19 +626,25 @@
 - Konzeptaufgaben thematisch in Pools sortieren (analog zum Dungeon)</t>
   </si>
   <si>
+    <t>Konzeptübungen (Abgabe/Vorstellung)</t>
+  </si>
+  <si>
+    <t>Dungeon-Aufgaben (Abgabe/Vorstellung)</t>
+  </si>
+  <si>
     <t>1 (Mo)</t>
   </si>
   <si>
     <t>kein Praktikum in W1</t>
   </si>
   <si>
-    <t>1 (Fr)</t>
+    <t>2 (Fr)</t>
   </si>
   <si>
     <r>
       <rPr>
         <rFont val="Helvetica Neue"/>
-        <color theme="1"/>
+        <color rgb="FF6AA84F"/>
       </rPr>
       <t xml:space="preserve">K1: Git (Basics, Branches, Remotes) 
 </t>
@@ -647,7 +653,7 @@
       <rPr>
         <rFont val="Helvetica Neue"/>
         <b/>
-        <color theme="1"/>
+        <color rgb="FF6AA84F"/>
       </rPr>
       <t>(nur Abgabe)</t>
     </r>
@@ -656,7 +662,7 @@
     <r>
       <rPr>
         <rFont val="Helvetica Neue"/>
-        <color theme="1"/>
+        <color rgb="FF6AA84F"/>
       </rPr>
       <t xml:space="preserve">K2: Logging, Factory-Method
 </t>
@@ -665,19 +671,55 @@
       <rPr>
         <rFont val="Helvetica Neue"/>
         <b/>
-        <color theme="1"/>
+        <color rgb="FF6AA84F"/>
       </rPr>
       <t>plus Vorstellung K1</t>
     </r>
   </si>
   <si>
+    <t>D1: Dungeon-Basics</t>
+  </si>
+  <si>
+    <t>JUnit1: Intro</t>
+  </si>
+  <si>
+    <t>JUnit2: Basics</t>
+  </si>
+  <si>
+    <t>JUnit3: Testfall-Ermittlung</t>
+  </si>
+  <si>
     <t>K3: Generics, Strategy</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Bad Smells</t>
+  </si>
+  <si>
+    <t>Coding Rules und Metriken</t>
+  </si>
+  <si>
+    <t>JUnit4: Mocking (Mockito)</t>
   </si>
   <si>
     <t>K4: Junit, Gradle</t>
   </si>
   <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>Serialisierung (equals, hashCode Wdhlg)</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
     <t>K6: Serialisierung, Type Object, Flyweight, Observer</t>
+  </si>
+  <si>
+    <t>D5</t>
   </si>
   <si>
     <t>Frameworks (Guava, Apache Commons, JDBC/?), ...)</t>
@@ -686,7 +728,31 @@
     <t>K7: Template-Method, Reflection, Annotations, Swing</t>
   </si>
   <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
     <t>K9: Stream-API, Optional, Visitor, Command-Pattern</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>E2 (tbd)</t>
+  </si>
+  <si>
+    <t>1 (Fr)</t>
   </si>
   <si>
     <r>
@@ -741,7 +807,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="18">
+  <fonts count="25">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -807,7 +873,42 @@
     </font>
     <font>
       <u/>
+      <color rgb="FF6AA84F"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF6AA84F"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF6AA84F"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF6AA84F"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF6AA84F"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FFFF9900"/>
       <name val="Helvetica Neue"/>
       <scheme val="minor"/>
     </font>
@@ -819,6 +920,12 @@
     </font>
     <font>
       <b/>
+      <u/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
@@ -1021,7 +1128,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="84">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1184,6 +1291,15 @@
     <xf borderId="0" fillId="9" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="9" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1193,25 +1309,55 @@
     <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -1220,19 +1366,19 @@
     <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -34898,14 +35044,14 @@
       <c r="D4" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="28">
-        <v>20.0</v>
+      <c r="E4" s="30">
+        <v>10.0</v>
       </c>
       <c r="F4" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="28">
-        <v>20.0</v>
+      <c r="G4" s="30">
+        <v>15.0</v>
       </c>
       <c r="H4" s="40" t="s">
         <v>66</v>
@@ -34933,7 +35079,7 @@
       </c>
       <c r="Q4" s="29">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="S4" s="30">
         <v>16.0</v>
@@ -38096,10 +38242,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
@@ -38114,9 +38257,10 @@
     <col customWidth="1" min="14" max="14" width="12.86"/>
     <col customWidth="1" min="15" max="15" width="8.14"/>
     <col customWidth="1" min="16" max="16" width="5.29"/>
+    <col customWidth="1" min="18" max="18" width="5.71"/>
     <col customWidth="1" min="19" max="19" width="6.14"/>
-    <col customWidth="1" min="20" max="20" width="14.0"/>
-    <col customWidth="1" min="21" max="22" width="48.86"/>
+    <col customWidth="1" min="20" max="20" width="13.29"/>
+    <col customWidth="1" min="21" max="22" width="44.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -38177,127 +38321,127 @@
         <v>130</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="54">
-        <v>40.0</v>
+        <v>45.0</v>
       </c>
       <c r="D2" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="54">
+      <c r="E2" s="55">
         <v>20.0</v>
       </c>
       <c r="F2" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="54">
+      <c r="G2" s="55">
         <v>25.0</v>
       </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="59"/>
       <c r="Q2" s="29">
         <f t="shared" ref="Q2:Q17" si="1">SUM(C2,E2,G2,I2,K2,M2,O2)</f>
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S2" s="30">
         <v>14.0</v>
       </c>
       <c r="T2" s="31"/>
       <c r="U2" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="V2" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="26" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B3" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="55">
         <v>25.0</v>
       </c>
       <c r="D3" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="55">
+      <c r="E3" s="54">
         <v>15.0</v>
       </c>
       <c r="F3" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="54">
+      <c r="G3" s="55">
         <v>25.0</v>
       </c>
       <c r="H3" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="54">
+      <c r="I3" s="55">
         <v>10.0</v>
       </c>
       <c r="J3" s="53" t="s">
         <v>52</v>
       </c>
       <c r="K3" s="54">
-        <v>15.0</v>
-      </c>
-      <c r="L3" s="56"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="56"/>
+        <v>20.0</v>
+      </c>
+      <c r="L3" s="59"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="59"/>
       <c r="Q3" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="S3" s="30">
         <v>14.0</v>
       </c>
       <c r="T3" s="31"/>
       <c r="U3" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="V3" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="61">
         <v>20.0</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="46">
-        <v>10.0</v>
+      <c r="E4" s="61">
+        <v>15.0</v>
       </c>
       <c r="F4" s="45"/>
       <c r="G4" s="46"/>
@@ -38320,68 +38464,68 @@
       <c r="P4" s="35"/>
       <c r="Q4" s="29">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="S4" s="30">
         <v>15.0</v>
       </c>
-      <c r="T4" s="57" t="s">
+      <c r="T4" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="U4" s="31" t="s">
-        <v>200</v>
+      <c r="U4" s="63" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="26" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B5" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="55">
         <v>20.0</v>
       </c>
       <c r="D5" s="53" t="s">
         <v>62</v>
       </c>
       <c r="E5" s="54">
-        <v>20.0</v>
+        <v>10.0</v>
       </c>
       <c r="F5" s="53" t="s">
         <v>63</v>
       </c>
       <c r="G5" s="54">
-        <v>20.0</v>
+        <v>15.0</v>
       </c>
       <c r="H5" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="54">
+      <c r="I5" s="55">
         <v>15.0</v>
       </c>
       <c r="J5" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="54">
+      <c r="K5" s="55">
         <v>10.0</v>
       </c>
-      <c r="L5" s="56" t="s">
+      <c r="L5" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M5" s="54" t="s">
+      <c r="M5" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N5" s="56" t="s">
+      <c r="N5" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O5" s="54" t="s">
+      <c r="O5" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P5" s="56"/>
+      <c r="P5" s="59"/>
       <c r="Q5" s="29">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="S5" s="30">
         <v>16.0</v>
@@ -38389,53 +38533,49 @@
       <c r="T5" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="U5" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="V5" s="31" t="s">
-        <v>183</v>
+      <c r="U5" s="63" t="s">
+        <v>203</v>
+      </c>
+      <c r="V5" s="63" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="B6" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="61">
+        <v>20.0</v>
+      </c>
+      <c r="D6" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="61">
+        <v>10.0</v>
+      </c>
+      <c r="F6" s="65" t="s">
+        <v>205</v>
+      </c>
+      <c r="G6" s="61">
+        <v>25.0</v>
+      </c>
+      <c r="H6" s="65" t="s">
+        <v>206</v>
+      </c>
+      <c r="I6" s="61">
+        <v>20.0</v>
+      </c>
+      <c r="J6" s="65" t="s">
+        <v>207</v>
+      </c>
+      <c r="K6" s="61">
         <v>15.0</v>
       </c>
-      <c r="D6" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6" s="34">
-        <v>20.0</v>
-      </c>
-      <c r="F6" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="34">
-        <v>20.0</v>
-      </c>
-      <c r="H6" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6" s="34">
-        <v>20.0</v>
-      </c>
-      <c r="J6" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="K6" s="34">
-        <v>15.0</v>
-      </c>
-      <c r="L6" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="M6" s="34" t="s">
-        <v>181</v>
-      </c>
+      <c r="L6" s="64"/>
+      <c r="M6" s="61"/>
       <c r="N6" s="35" t="s">
         <v>181</v>
       </c>
@@ -38451,176 +38591,180 @@
         <v>17.0</v>
       </c>
       <c r="T6" s="31"/>
-      <c r="U6" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="V6" s="31" t="s">
-        <v>142</v>
+      <c r="U6" s="63" t="s">
+        <v>208</v>
+      </c>
+      <c r="V6" s="63" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="B7" s="53" t="s">
-        <v>55</v>
+        <v>149</v>
+      </c>
+      <c r="B7" s="66" t="s">
+        <v>210</v>
       </c>
       <c r="C7" s="54">
-        <v>35.0</v>
-      </c>
-      <c r="D7" s="53" t="s">
+        <v>30.0</v>
+      </c>
+      <c r="D7" s="66" t="s">
+        <v>211</v>
+      </c>
+      <c r="E7" s="54">
+        <v>30.0</v>
+      </c>
+      <c r="F7" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="54">
-        <v>35.0</v>
-      </c>
-      <c r="F7" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="59">
+      <c r="G7" s="54">
         <v>20.0</v>
       </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="56" t="s">
+      <c r="H7" s="67" t="s">
+        <v>212</v>
+      </c>
+      <c r="I7" s="68">
+        <v>20.0</v>
+      </c>
+      <c r="J7" s="69"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M7" s="54" t="s">
+      <c r="M7" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N7" s="56" t="s">
+      <c r="N7" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O7" s="54" t="s">
+      <c r="O7" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P7" s="56"/>
+      <c r="P7" s="59"/>
       <c r="Q7" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="S7" s="30">
         <v>18.0</v>
       </c>
       <c r="T7" s="31"/>
-      <c r="U7" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="V7" s="31" t="s">
-        <v>145</v>
+      <c r="U7" s="63" t="s">
+        <v>213</v>
+      </c>
+      <c r="V7" s="63" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="B8" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="61">
         <v>5.0</v>
       </c>
-      <c r="D8" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="46">
+      <c r="D8" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="61">
+        <v>15.0</v>
+      </c>
+      <c r="F8" s="70" t="s">
+        <v>215</v>
+      </c>
+      <c r="G8" s="46">
         <v>20.0</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="H8" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="60">
+      <c r="I8" s="71">
         <v>25.0</v>
       </c>
-      <c r="H8" s="47" t="s">
+      <c r="J8" s="47" t="s">
         <v>43</v>
-      </c>
-      <c r="I8" s="46">
-        <v>10.0</v>
-      </c>
-      <c r="J8" s="47" t="s">
-        <v>44</v>
       </c>
       <c r="K8" s="46">
         <v>10.0</v>
       </c>
-      <c r="L8" s="45" t="s">
-        <v>32</v>
+      <c r="L8" s="47" t="s">
+        <v>44</v>
       </c>
       <c r="M8" s="46">
         <v>10.0</v>
       </c>
-      <c r="N8" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="O8" s="34" t="s">
-        <v>181</v>
+      <c r="N8" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="46">
+        <v>10.0</v>
       </c>
       <c r="P8" s="35"/>
       <c r="Q8" s="29">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="S8" s="30">
         <v>19.0</v>
       </c>
       <c r="T8" s="31"/>
-      <c r="U8" s="31" t="s">
+      <c r="U8" s="63" t="s">
         <v>187</v>
       </c>
-      <c r="V8" s="31" t="s">
-        <v>148</v>
+      <c r="V8" s="63" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="B9" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="57">
         <v>30.0</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="57">
         <v>30.0</v>
       </c>
-      <c r="F9" s="61" t="s">
+      <c r="F9" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="59">
+      <c r="G9" s="68">
         <v>15.0</v>
       </c>
-      <c r="H9" s="56" t="s">
+      <c r="H9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="I9" s="54" t="s">
+      <c r="I9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="J9" s="56" t="s">
+      <c r="J9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="K9" s="54" t="s">
+      <c r="K9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="L9" s="56" t="s">
+      <c r="L9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M9" s="54" t="s">
+      <c r="M9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N9" s="56" t="s">
+      <c r="N9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O9" s="54" t="s">
+      <c r="O9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P9" s="56"/>
+      <c r="P9" s="59"/>
       <c r="Q9" s="29">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -38630,24 +38774,24 @@
       </c>
       <c r="T9" s="31"/>
       <c r="U9" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="V9" s="31" t="s">
-        <v>151</v>
+        <v>217</v>
+      </c>
+      <c r="V9" s="63" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" s="62" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="73" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="34">
         <v>45.0</v>
       </c>
-      <c r="D10" s="63" t="s">
-        <v>205</v>
+      <c r="D10" s="74" t="s">
+        <v>219</v>
       </c>
       <c r="E10" s="46">
         <v>25.0</v>
@@ -38702,43 +38846,43 @@
     </row>
     <row r="11">
       <c r="A11" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" s="53" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="54">
+      <c r="C11" s="57">
         <v>10.0</v>
       </c>
-      <c r="D11" s="53" t="s">
+      <c r="D11" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="54">
+      <c r="E11" s="57">
         <v>25.0</v>
       </c>
-      <c r="F11" s="53" t="s">
+      <c r="F11" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="54">
+      <c r="G11" s="57">
         <v>20.0</v>
       </c>
-      <c r="H11" s="53" t="s">
+      <c r="H11" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="54">
+      <c r="I11" s="57">
         <v>35.0</v>
       </c>
-      <c r="J11" s="58"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="56" t="s">
+      <c r="J11" s="75"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O11" s="54" t="s">
+      <c r="O11" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P11" s="56"/>
+      <c r="P11" s="59"/>
       <c r="Q11" s="29">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -38748,15 +38892,15 @@
       </c>
       <c r="T11" s="31"/>
       <c r="U11" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="V11" s="31" t="s">
-        <v>154</v>
+        <v>220</v>
+      </c>
+      <c r="V11" s="63" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="26" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B12" s="47" t="s">
         <v>74</v>
@@ -38814,57 +38958,57 @@
       <c r="U12" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="V12" s="31" t="s">
-        <v>160</v>
+      <c r="V12" s="63" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="B13" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="57">
         <v>10.0</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="57">
         <v>25.0</v>
       </c>
-      <c r="F13" s="56" t="s">
+      <c r="F13" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="54">
+      <c r="G13" s="57">
         <v>25.0</v>
       </c>
-      <c r="H13" s="53" t="s">
+      <c r="H13" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="54">
+      <c r="I13" s="57">
         <v>15.0</v>
       </c>
-      <c r="J13" s="58" t="s">
+      <c r="J13" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="K13" s="59">
+      <c r="K13" s="68">
         <v>15.0</v>
       </c>
-      <c r="L13" s="56" t="s">
+      <c r="L13" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M13" s="54" t="s">
+      <c r="M13" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N13" s="56" t="s">
+      <c r="N13" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O13" s="54" t="s">
+      <c r="O13" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P13" s="56"/>
+      <c r="P13" s="59"/>
       <c r="Q13" s="29">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -38876,15 +39020,15 @@
         <v>166</v>
       </c>
       <c r="U13" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="V13" s="31" t="s">
-        <v>164</v>
+        <v>223</v>
+      </c>
+      <c r="V13" s="63" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="26" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B14" s="47" t="s">
         <v>81</v>
@@ -38936,57 +39080,57 @@
       <c r="U14" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="V14" s="31" t="s">
-        <v>168</v>
+      <c r="V14" s="63" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="B15" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="54">
+      <c r="C15" s="57">
         <v>20.0</v>
       </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="54">
+      <c r="E15" s="57">
         <v>20.0</v>
       </c>
-      <c r="F15" s="56" t="s">
+      <c r="F15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="H15" s="56" t="s">
+      <c r="H15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="I15" s="54" t="s">
+      <c r="I15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="56" t="s">
+      <c r="J15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="K15" s="54" t="s">
+      <c r="K15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="56" t="s">
+      <c r="L15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M15" s="54" t="s">
+      <c r="M15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N15" s="56" t="s">
+      <c r="N15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O15" s="54" t="s">
+      <c r="O15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P15" s="56"/>
+      <c r="P15" s="59"/>
       <c r="Q15" s="29">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -38994,13 +39138,13 @@
       <c r="S15" s="30">
         <v>26.0</v>
       </c>
-      <c r="V15" s="31" t="s">
-        <v>171</v>
+      <c r="V15" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="26" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B16" s="37" t="s">
         <v>181</v>
@@ -39055,10 +39199,10 @@
     </row>
     <row r="17">
       <c r="A17" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="B17" s="49" t="s">
-        <v>112</v>
+        <v>227</v>
+      </c>
+      <c r="B17" s="76" t="s">
+        <v>228</v>
       </c>
       <c r="C17" s="38">
         <v>45.0</v>
@@ -39122,10 +39266,10 @@
     </row>
     <row r="20">
       <c r="A20" s="4"/>
-      <c r="D20" s="64" t="s">
+      <c r="D20" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="65">
+      <c r="E20" s="78">
         <v>15.0</v>
       </c>
       <c r="S20" s="31"/>
@@ -39140,10 +39284,10 @@
     </row>
     <row r="21">
       <c r="A21" s="4"/>
-      <c r="D21" s="64" t="s">
+      <c r="D21" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="65">
+      <c r="E21" s="78">
         <v>20.0</v>
       </c>
       <c r="S21" s="31"/>
@@ -41633,35 +41777,35 @@
     </row>
     <row r="2">
       <c r="A2" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="B2" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="54">
+      <c r="C2" s="57">
         <v>40.0</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="54">
+      <c r="E2" s="57">
         <v>20.0</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="54">
+      <c r="G2" s="57">
         <v>25.0</v>
       </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="59"/>
       <c r="Q2" s="29">
         <f t="shared" ref="Q2:Q17" si="1">SUM(C2,E2,G2,I2,K2,M2,O2)</f>
         <v>85</v>
@@ -41671,47 +41815,47 @@
       </c>
       <c r="T2" s="31"/>
       <c r="U2" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="V2" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="B3" s="53" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="57">
         <v>25.0</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="55">
+      <c r="E3" s="58">
         <v>15.0</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="54">
+      <c r="G3" s="57">
         <v>25.0</v>
       </c>
-      <c r="H3" s="53" t="s">
+      <c r="H3" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="55">
+      <c r="I3" s="58">
         <v>20.0</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="59"/>
       <c r="Q3" s="29">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -41721,10 +41865,10 @@
       </c>
       <c r="T3" s="31"/>
       <c r="U3" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="V3" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4">
@@ -41761,63 +41905,63 @@
       <c r="S4" s="30">
         <v>15.0</v>
       </c>
-      <c r="T4" s="57" t="s">
+      <c r="T4" s="62" t="s">
         <v>136</v>
       </c>
       <c r="U4" s="31" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="57">
         <v>20.0</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="54">
-        <v>20.0</v>
-      </c>
-      <c r="F5" s="53" t="s">
+      <c r="E5" s="58">
+        <v>10.0</v>
+      </c>
+      <c r="F5" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="54">
+      <c r="G5" s="57">
         <v>15.0</v>
       </c>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="54">
+      <c r="I5" s="57">
         <v>10.0</v>
       </c>
-      <c r="J5" s="66" t="s">
+      <c r="J5" s="79" t="s">
         <v>98</v>
       </c>
-      <c r="K5" s="67">
+      <c r="K5" s="80">
         <v>15.0</v>
       </c>
-      <c r="L5" s="61" t="s">
+      <c r="L5" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="M5" s="59">
+      <c r="M5" s="68">
         <v>10.0</v>
       </c>
-      <c r="N5" s="56" t="s">
+      <c r="N5" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O5" s="54" t="s">
+      <c r="O5" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P5" s="56"/>
+      <c r="P5" s="59"/>
       <c r="Q5" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="S5" s="30">
         <v>16.0</v>
@@ -41825,8 +41969,8 @@
       <c r="T5" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="U5" s="68" t="s">
-        <v>209</v>
+      <c r="U5" s="81" t="s">
+        <v>231</v>
       </c>
       <c r="V5" s="31" t="s">
         <v>183</v>
@@ -41836,16 +41980,16 @@
       <c r="A6" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="70">
+      <c r="C6" s="83">
         <v>20.0</v>
       </c>
-      <c r="D6" s="69" t="s">
+      <c r="D6" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="70">
+      <c r="E6" s="83">
         <v>20.0</v>
       </c>
       <c r="F6" s="43" t="s">
@@ -41857,8 +42001,8 @@
       <c r="H6" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="I6" s="34">
-        <v>20.0</v>
+      <c r="I6" s="44">
+        <v>15.0</v>
       </c>
       <c r="J6" s="43" t="s">
         <v>66</v>
@@ -41881,14 +42025,14 @@
       <c r="P6" s="35"/>
       <c r="Q6" s="29">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="S6" s="30">
         <v>17.0</v>
       </c>
       <c r="T6" s="31"/>
       <c r="U6" s="31" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="V6" s="31" t="s">
         <v>142</v>
@@ -41898,41 +42042,41 @@
       <c r="A7" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="57">
         <v>35.0</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="54">
+      <c r="E7" s="57">
         <v>35.0</v>
       </c>
-      <c r="F7" s="58" t="s">
+      <c r="F7" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="59">
+      <c r="G7" s="68">
         <v>20.0</v>
       </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="56" t="s">
+      <c r="H7" s="75"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M7" s="54" t="s">
+      <c r="M7" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N7" s="56" t="s">
+      <c r="N7" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O7" s="54" t="s">
+      <c r="O7" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P7" s="56"/>
+      <c r="P7" s="59"/>
       <c r="Q7" s="29">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -41942,7 +42086,7 @@
       </c>
       <c r="T7" s="31"/>
       <c r="U7" s="31" t="s">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="V7" s="31" t="s">
         <v>145</v>
@@ -41973,7 +42117,7 @@
       <c r="H8" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="I8" s="60">
+      <c r="I8" s="71">
         <v>25.0</v>
       </c>
       <c r="J8" s="47" t="s">
@@ -42004,7 +42148,7 @@
       </c>
       <c r="T8" s="31"/>
       <c r="U8" s="31" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="V8" s="31" t="s">
         <v>148</v>
@@ -42014,49 +42158,49 @@
       <c r="A9" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="57">
         <v>30.0</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="57">
         <v>30.0</v>
       </c>
-      <c r="F9" s="61" t="s">
+      <c r="F9" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="59">
+      <c r="G9" s="68">
         <v>15.0</v>
       </c>
-      <c r="H9" s="56" t="s">
+      <c r="H9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="I9" s="54" t="s">
+      <c r="I9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="J9" s="56" t="s">
+      <c r="J9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="K9" s="54" t="s">
+      <c r="K9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="L9" s="56" t="s">
+      <c r="L9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M9" s="54" t="s">
+      <c r="M9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N9" s="56" t="s">
+      <c r="N9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O9" s="54" t="s">
+      <c r="O9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P9" s="56"/>
+      <c r="P9" s="59"/>
       <c r="Q9" s="29">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -42066,7 +42210,7 @@
       </c>
       <c r="T9" s="31"/>
       <c r="U9" s="31" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="V9" s="31" t="s">
         <v>151</v>
@@ -42076,14 +42220,14 @@
       <c r="A10" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="73" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="34">
         <v>45.0</v>
       </c>
-      <c r="D10" s="63" t="s">
-        <v>205</v>
+      <c r="D10" s="74" t="s">
+        <v>219</v>
       </c>
       <c r="E10" s="46">
         <v>25.0</v>
@@ -42140,41 +42284,41 @@
       <c r="A11" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="54">
+      <c r="C11" s="57">
         <v>10.0</v>
       </c>
-      <c r="D11" s="53" t="s">
+      <c r="D11" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="54">
+      <c r="E11" s="57">
         <v>25.0</v>
       </c>
-      <c r="F11" s="53" t="s">
+      <c r="F11" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="54">
+      <c r="G11" s="57">
         <v>20.0</v>
       </c>
-      <c r="H11" s="53" t="s">
+      <c r="H11" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="54">
+      <c r="I11" s="57">
         <v>35.0</v>
       </c>
-      <c r="J11" s="58"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="56" t="s">
+      <c r="J11" s="75"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O11" s="54" t="s">
+      <c r="O11" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P11" s="56"/>
+      <c r="P11" s="59"/>
       <c r="Q11" s="29">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -42184,7 +42328,7 @@
       </c>
       <c r="T11" s="31"/>
       <c r="U11" s="31" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="V11" s="31" t="s">
         <v>154</v>
@@ -42248,7 +42392,7 @@
         <v>162</v>
       </c>
       <c r="U12" s="31" t="s">
-        <v>215</v>
+        <v>237</v>
       </c>
       <c r="V12" s="31" t="s">
         <v>160</v>
@@ -42258,49 +42402,49 @@
       <c r="A13" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="57">
         <v>10.0</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="57">
         <v>25.0</v>
       </c>
-      <c r="F13" s="56" t="s">
+      <c r="F13" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="54">
+      <c r="G13" s="57">
         <v>25.0</v>
       </c>
-      <c r="H13" s="53" t="s">
+      <c r="H13" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="54">
+      <c r="I13" s="57">
         <v>15.0</v>
       </c>
-      <c r="J13" s="58" t="s">
+      <c r="J13" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="K13" s="59">
+      <c r="K13" s="68">
         <v>15.0</v>
       </c>
-      <c r="L13" s="56" t="s">
+      <c r="L13" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M13" s="54" t="s">
+      <c r="M13" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N13" s="56" t="s">
+      <c r="N13" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O13" s="54" t="s">
+      <c r="O13" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P13" s="56"/>
+      <c r="P13" s="59"/>
       <c r="Q13" s="29">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -42312,7 +42456,7 @@
         <v>166</v>
       </c>
       <c r="U13" s="31" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="V13" s="31" t="s">
         <v>164</v>
@@ -42370,7 +42514,7 @@
       </c>
       <c r="T14" s="31"/>
       <c r="U14" s="31" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="V14" s="31" t="s">
         <v>168</v>
@@ -42380,49 +42524,49 @@
       <c r="A15" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="54">
+      <c r="C15" s="57">
         <v>20.0</v>
       </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="54">
+      <c r="E15" s="57">
         <v>20.0</v>
       </c>
-      <c r="F15" s="56" t="s">
+      <c r="F15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="H15" s="56" t="s">
+      <c r="H15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="I15" s="54" t="s">
+      <c r="I15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="56" t="s">
+      <c r="J15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="K15" s="54" t="s">
+      <c r="K15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="56" t="s">
+      <c r="L15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M15" s="54" t="s">
+      <c r="M15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N15" s="56" t="s">
+      <c r="N15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O15" s="54" t="s">
+      <c r="O15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P15" s="56"/>
+      <c r="P15" s="59"/>
       <c r="Q15" s="29">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -42431,7 +42575,7 @@
         <v>26.0</v>
       </c>
       <c r="U15" s="31" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="V15" s="31" t="s">
         <v>171</v>
@@ -42561,10 +42705,10 @@
     </row>
     <row r="20">
       <c r="A20" s="4"/>
-      <c r="D20" s="64" t="s">
+      <c r="D20" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="65">
+      <c r="E20" s="78">
         <v>15.0</v>
       </c>
       <c r="S20" s="31"/>
@@ -42579,10 +42723,10 @@
     </row>
     <row r="21">
       <c r="A21" s="4"/>
-      <c r="D21" s="64" t="s">
+      <c r="D21" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="65">
+      <c r="E21" s="78">
         <v>20.0</v>
       </c>
       <c r="S21" s="31"/>
@@ -42594,16 +42738,16 @@
     </row>
     <row r="22">
       <c r="A22" s="4"/>
-      <c r="D22" s="64" t="s">
+      <c r="D22" s="77" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="65">
+      <c r="E22" s="78">
         <v>20.0</v>
       </c>
-      <c r="H22" s="56"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="54"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="57"/>
       <c r="S22" s="31"/>
       <c r="T22" s="31"/>
       <c r="U22" s="31"/>

</xml_diff>

<commit_message>
Update Schedule: move TDD to KW19 (#427)
</commit_message>
<xml_diff>
--- a/planung_pm.xlsx
+++ b/planung_pm.xlsx
@@ -5,9 +5,9 @@
   <sheets>
     <sheet state="hidden" name="Themen" sheetId="1" r:id="rId4"/>
     <sheet state="hidden" name="Wochenüberblick (alt Formeln)" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Wochenüberblick (alt VL Mo)" sheetId="3" r:id="rId6"/>
+    <sheet state="hidden" name="Wochenüberblick (alt VL Mo)" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="V1 (neu VL Fr)" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="V2 (neu VL Fr)" sheetId="5" r:id="rId8"/>
+    <sheet state="hidden" name="V2 (neu VL Fr)" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="241">
   <si>
     <t>Thema</t>
   </si>
@@ -626,19 +626,25 @@
 - Konzeptaufgaben thematisch in Pools sortieren (analog zum Dungeon)</t>
   </si>
   <si>
+    <t>Konzeptübungen (Abgabe/Vorstellung)</t>
+  </si>
+  <si>
+    <t>Dungeon-Aufgaben (Abgabe/Vorstellung)</t>
+  </si>
+  <si>
     <t>1 (Mo)</t>
   </si>
   <si>
     <t>kein Praktikum in W1</t>
   </si>
   <si>
-    <t>1 (Fr)</t>
+    <t>2 (Fr)</t>
   </si>
   <si>
     <r>
       <rPr>
         <rFont val="Helvetica Neue"/>
-        <color theme="1"/>
+        <color rgb="FF6AA84F"/>
       </rPr>
       <t xml:space="preserve">K1: Git (Basics, Branches, Remotes) 
 </t>
@@ -647,7 +653,7 @@
       <rPr>
         <rFont val="Helvetica Neue"/>
         <b/>
-        <color theme="1"/>
+        <color rgb="FF6AA84F"/>
       </rPr>
       <t>(nur Abgabe)</t>
     </r>
@@ -656,7 +662,7 @@
     <r>
       <rPr>
         <rFont val="Helvetica Neue"/>
-        <color theme="1"/>
+        <color rgb="FF6AA84F"/>
       </rPr>
       <t xml:space="preserve">K2: Logging, Factory-Method
 </t>
@@ -665,19 +671,55 @@
       <rPr>
         <rFont val="Helvetica Neue"/>
         <b/>
-        <color theme="1"/>
+        <color rgb="FF6AA84F"/>
       </rPr>
       <t>plus Vorstellung K1</t>
     </r>
   </si>
   <si>
+    <t>D1: Dungeon-Basics</t>
+  </si>
+  <si>
+    <t>JUnit1: Intro</t>
+  </si>
+  <si>
+    <t>JUnit2: Basics</t>
+  </si>
+  <si>
+    <t>JUnit3: Testfall-Ermittlung</t>
+  </si>
+  <si>
     <t>K3: Generics, Strategy</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Bad Smells</t>
+  </si>
+  <si>
+    <t>Coding Rules und Metriken</t>
+  </si>
+  <si>
+    <t>JUnit4: Mocking (Mockito)</t>
   </si>
   <si>
     <t>K4: Junit, Gradle</t>
   </si>
   <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>Serialisierung (equals, hashCode Wdhlg)</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
     <t>K6: Serialisierung, Type Object, Flyweight, Observer</t>
+  </si>
+  <si>
+    <t>D5</t>
   </si>
   <si>
     <t>Frameworks (Guava, Apache Commons, JDBC/?), ...)</t>
@@ -686,7 +728,31 @@
     <t>K7: Template-Method, Reflection, Annotations, Swing</t>
   </si>
   <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
     <t>K9: Stream-API, Optional, Visitor, Command-Pattern</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>E2 (tbd)</t>
+  </si>
+  <si>
+    <t>1 (Fr)</t>
   </si>
   <si>
     <r>
@@ -741,7 +807,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="18">
+  <fonts count="25">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -807,7 +873,42 @@
     </font>
     <font>
       <u/>
+      <color rgb="FF6AA84F"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF6AA84F"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF6AA84F"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF6AA84F"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF6AA84F"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FFFF9900"/>
       <name val="Helvetica Neue"/>
       <scheme val="minor"/>
     </font>
@@ -819,6 +920,12 @@
     </font>
     <font>
       <b/>
+      <u/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
@@ -1021,7 +1128,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="84">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1184,6 +1291,15 @@
     <xf borderId="0" fillId="9" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="9" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1193,25 +1309,55 @@
     <xf borderId="0" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -1220,19 +1366,19 @@
     <xf borderId="0" fillId="10" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -34898,14 +35044,14 @@
       <c r="D4" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="28">
-        <v>20.0</v>
+      <c r="E4" s="30">
+        <v>10.0</v>
       </c>
       <c r="F4" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="28">
-        <v>20.0</v>
+      <c r="G4" s="30">
+        <v>15.0</v>
       </c>
       <c r="H4" s="40" t="s">
         <v>66</v>
@@ -34933,7 +35079,7 @@
       </c>
       <c r="Q4" s="29">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="S4" s="30">
         <v>16.0</v>
@@ -38096,10 +38242,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
@@ -38114,9 +38257,10 @@
     <col customWidth="1" min="14" max="14" width="12.86"/>
     <col customWidth="1" min="15" max="15" width="8.14"/>
     <col customWidth="1" min="16" max="16" width="5.29"/>
+    <col customWidth="1" min="18" max="18" width="5.71"/>
     <col customWidth="1" min="19" max="19" width="6.14"/>
-    <col customWidth="1" min="20" max="20" width="14.0"/>
-    <col customWidth="1" min="21" max="22" width="48.86"/>
+    <col customWidth="1" min="20" max="20" width="13.29"/>
+    <col customWidth="1" min="21" max="22" width="44.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -38177,127 +38321,127 @@
         <v>130</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="26" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="54">
-        <v>40.0</v>
+        <v>45.0</v>
       </c>
       <c r="D2" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="54">
+      <c r="E2" s="55">
         <v>20.0</v>
       </c>
       <c r="F2" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="54">
+      <c r="G2" s="55">
         <v>25.0</v>
       </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="59"/>
       <c r="Q2" s="29">
         <f t="shared" ref="Q2:Q17" si="1">SUM(C2,E2,G2,I2,K2,M2,O2)</f>
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="S2" s="30">
         <v>14.0</v>
       </c>
       <c r="T2" s="31"/>
       <c r="U2" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="V2" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="26" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B3" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="55">
         <v>25.0</v>
       </c>
       <c r="D3" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="55">
+      <c r="E3" s="54">
         <v>15.0</v>
       </c>
       <c r="F3" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="54">
+      <c r="G3" s="55">
         <v>25.0</v>
       </c>
       <c r="H3" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="54">
+      <c r="I3" s="55">
         <v>10.0</v>
       </c>
       <c r="J3" s="53" t="s">
         <v>52</v>
       </c>
       <c r="K3" s="54">
-        <v>15.0</v>
-      </c>
-      <c r="L3" s="56"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="56"/>
+        <v>20.0</v>
+      </c>
+      <c r="L3" s="59"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="59"/>
       <c r="Q3" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="S3" s="30">
         <v>14.0</v>
       </c>
       <c r="T3" s="31"/>
       <c r="U3" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="V3" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="61">
         <v>20.0</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="46">
-        <v>10.0</v>
+      <c r="E4" s="61">
+        <v>15.0</v>
       </c>
       <c r="F4" s="45"/>
       <c r="G4" s="46"/>
@@ -38320,68 +38464,68 @@
       <c r="P4" s="35"/>
       <c r="Q4" s="29">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="S4" s="30">
         <v>15.0</v>
       </c>
-      <c r="T4" s="57" t="s">
+      <c r="T4" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="U4" s="31" t="s">
-        <v>200</v>
+      <c r="U4" s="63" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="26" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B5" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="55">
         <v>20.0</v>
       </c>
       <c r="D5" s="53" t="s">
         <v>62</v>
       </c>
       <c r="E5" s="54">
-        <v>20.0</v>
+        <v>10.0</v>
       </c>
       <c r="F5" s="53" t="s">
         <v>63</v>
       </c>
       <c r="G5" s="54">
-        <v>20.0</v>
+        <v>15.0</v>
       </c>
       <c r="H5" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="54">
+      <c r="I5" s="55">
         <v>15.0</v>
       </c>
       <c r="J5" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="54">
+      <c r="K5" s="55">
         <v>10.0</v>
       </c>
-      <c r="L5" s="56" t="s">
+      <c r="L5" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M5" s="54" t="s">
+      <c r="M5" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N5" s="56" t="s">
+      <c r="N5" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O5" s="54" t="s">
+      <c r="O5" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P5" s="56"/>
+      <c r="P5" s="59"/>
       <c r="Q5" s="29">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="S5" s="30">
         <v>16.0</v>
@@ -38389,53 +38533,49 @@
       <c r="T5" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="U5" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="V5" s="31" t="s">
-        <v>183</v>
+      <c r="U5" s="63" t="s">
+        <v>203</v>
+      </c>
+      <c r="V5" s="63" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="B6" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="61">
+        <v>20.0</v>
+      </c>
+      <c r="D6" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="61">
+        <v>10.0</v>
+      </c>
+      <c r="F6" s="65" t="s">
+        <v>205</v>
+      </c>
+      <c r="G6" s="61">
+        <v>25.0</v>
+      </c>
+      <c r="H6" s="65" t="s">
+        <v>206</v>
+      </c>
+      <c r="I6" s="61">
+        <v>20.0</v>
+      </c>
+      <c r="J6" s="65" t="s">
+        <v>207</v>
+      </c>
+      <c r="K6" s="61">
         <v>15.0</v>
       </c>
-      <c r="D6" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6" s="34">
-        <v>20.0</v>
-      </c>
-      <c r="F6" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="34">
-        <v>20.0</v>
-      </c>
-      <c r="H6" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6" s="34">
-        <v>20.0</v>
-      </c>
-      <c r="J6" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="K6" s="34">
-        <v>15.0</v>
-      </c>
-      <c r="L6" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="M6" s="34" t="s">
-        <v>181</v>
-      </c>
+      <c r="L6" s="64"/>
+      <c r="M6" s="61"/>
       <c r="N6" s="35" t="s">
         <v>181</v>
       </c>
@@ -38451,176 +38591,180 @@
         <v>17.0</v>
       </c>
       <c r="T6" s="31"/>
-      <c r="U6" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="V6" s="31" t="s">
-        <v>142</v>
+      <c r="U6" s="63" t="s">
+        <v>208</v>
+      </c>
+      <c r="V6" s="63" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="B7" s="53" t="s">
-        <v>55</v>
+        <v>149</v>
+      </c>
+      <c r="B7" s="66" t="s">
+        <v>210</v>
       </c>
       <c r="C7" s="54">
-        <v>35.0</v>
-      </c>
-      <c r="D7" s="53" t="s">
+        <v>30.0</v>
+      </c>
+      <c r="D7" s="66" t="s">
+        <v>211</v>
+      </c>
+      <c r="E7" s="54">
+        <v>30.0</v>
+      </c>
+      <c r="F7" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="54">
-        <v>35.0</v>
-      </c>
-      <c r="F7" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="59">
+      <c r="G7" s="54">
         <v>20.0</v>
       </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="56" t="s">
+      <c r="H7" s="67" t="s">
+        <v>212</v>
+      </c>
+      <c r="I7" s="68">
+        <v>20.0</v>
+      </c>
+      <c r="J7" s="69"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M7" s="54" t="s">
+      <c r="M7" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N7" s="56" t="s">
+      <c r="N7" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O7" s="54" t="s">
+      <c r="O7" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P7" s="56"/>
+      <c r="P7" s="59"/>
       <c r="Q7" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="S7" s="30">
         <v>18.0</v>
       </c>
       <c r="T7" s="31"/>
-      <c r="U7" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="V7" s="31" t="s">
-        <v>145</v>
+      <c r="U7" s="63" t="s">
+        <v>213</v>
+      </c>
+      <c r="V7" s="63" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="B8" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="61">
         <v>5.0</v>
       </c>
-      <c r="D8" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="46">
+      <c r="D8" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="61">
+        <v>15.0</v>
+      </c>
+      <c r="F8" s="70" t="s">
+        <v>215</v>
+      </c>
+      <c r="G8" s="46">
         <v>20.0</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="H8" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="60">
+      <c r="I8" s="71">
         <v>25.0</v>
       </c>
-      <c r="H8" s="47" t="s">
+      <c r="J8" s="47" t="s">
         <v>43</v>
-      </c>
-      <c r="I8" s="46">
-        <v>10.0</v>
-      </c>
-      <c r="J8" s="47" t="s">
-        <v>44</v>
       </c>
       <c r="K8" s="46">
         <v>10.0</v>
       </c>
-      <c r="L8" s="45" t="s">
-        <v>32</v>
+      <c r="L8" s="47" t="s">
+        <v>44</v>
       </c>
       <c r="M8" s="46">
         <v>10.0</v>
       </c>
-      <c r="N8" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="O8" s="34" t="s">
-        <v>181</v>
+      <c r="N8" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="46">
+        <v>10.0</v>
       </c>
       <c r="P8" s="35"/>
       <c r="Q8" s="29">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="S8" s="30">
         <v>19.0</v>
       </c>
       <c r="T8" s="31"/>
-      <c r="U8" s="31" t="s">
+      <c r="U8" s="63" t="s">
         <v>187</v>
       </c>
-      <c r="V8" s="31" t="s">
-        <v>148</v>
+      <c r="V8" s="63" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="B9" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="57">
         <v>30.0</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="57">
         <v>30.0</v>
       </c>
-      <c r="F9" s="61" t="s">
+      <c r="F9" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="59">
+      <c r="G9" s="68">
         <v>15.0</v>
       </c>
-      <c r="H9" s="56" t="s">
+      <c r="H9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="I9" s="54" t="s">
+      <c r="I9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="J9" s="56" t="s">
+      <c r="J9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="K9" s="54" t="s">
+      <c r="K9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="L9" s="56" t="s">
+      <c r="L9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M9" s="54" t="s">
+      <c r="M9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N9" s="56" t="s">
+      <c r="N9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O9" s="54" t="s">
+      <c r="O9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P9" s="56"/>
+      <c r="P9" s="59"/>
       <c r="Q9" s="29">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -38630,24 +38774,24 @@
       </c>
       <c r="T9" s="31"/>
       <c r="U9" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="V9" s="31" t="s">
-        <v>151</v>
+        <v>217</v>
+      </c>
+      <c r="V9" s="63" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" s="62" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="73" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="34">
         <v>45.0</v>
       </c>
-      <c r="D10" s="63" t="s">
-        <v>205</v>
+      <c r="D10" s="74" t="s">
+        <v>219</v>
       </c>
       <c r="E10" s="46">
         <v>25.0</v>
@@ -38702,43 +38846,43 @@
     </row>
     <row r="11">
       <c r="A11" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" s="53" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="54">
+      <c r="C11" s="57">
         <v>10.0</v>
       </c>
-      <c r="D11" s="53" t="s">
+      <c r="D11" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="54">
+      <c r="E11" s="57">
         <v>25.0</v>
       </c>
-      <c r="F11" s="53" t="s">
+      <c r="F11" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="54">
+      <c r="G11" s="57">
         <v>20.0</v>
       </c>
-      <c r="H11" s="53" t="s">
+      <c r="H11" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="54">
+      <c r="I11" s="57">
         <v>35.0</v>
       </c>
-      <c r="J11" s="58"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="56" t="s">
+      <c r="J11" s="75"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O11" s="54" t="s">
+      <c r="O11" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P11" s="56"/>
+      <c r="P11" s="59"/>
       <c r="Q11" s="29">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -38748,15 +38892,15 @@
       </c>
       <c r="T11" s="31"/>
       <c r="U11" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="V11" s="31" t="s">
-        <v>154</v>
+        <v>220</v>
+      </c>
+      <c r="V11" s="63" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="26" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B12" s="47" t="s">
         <v>74</v>
@@ -38814,57 +38958,57 @@
       <c r="U12" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="V12" s="31" t="s">
-        <v>160</v>
+      <c r="V12" s="63" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="B13" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="57">
         <v>10.0</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="57">
         <v>25.0</v>
       </c>
-      <c r="F13" s="56" t="s">
+      <c r="F13" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="54">
+      <c r="G13" s="57">
         <v>25.0</v>
       </c>
-      <c r="H13" s="53" t="s">
+      <c r="H13" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="54">
+      <c r="I13" s="57">
         <v>15.0</v>
       </c>
-      <c r="J13" s="58" t="s">
+      <c r="J13" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="K13" s="59">
+      <c r="K13" s="68">
         <v>15.0</v>
       </c>
-      <c r="L13" s="56" t="s">
+      <c r="L13" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M13" s="54" t="s">
+      <c r="M13" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N13" s="56" t="s">
+      <c r="N13" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O13" s="54" t="s">
+      <c r="O13" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P13" s="56"/>
+      <c r="P13" s="59"/>
       <c r="Q13" s="29">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -38876,15 +39020,15 @@
         <v>166</v>
       </c>
       <c r="U13" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="V13" s="31" t="s">
-        <v>164</v>
+        <v>223</v>
+      </c>
+      <c r="V13" s="63" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="26" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B14" s="47" t="s">
         <v>81</v>
@@ -38936,57 +39080,57 @@
       <c r="U14" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="V14" s="31" t="s">
-        <v>168</v>
+      <c r="V14" s="63" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="B15" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="54">
+      <c r="C15" s="57">
         <v>20.0</v>
       </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="54">
+      <c r="E15" s="57">
         <v>20.0</v>
       </c>
-      <c r="F15" s="56" t="s">
+      <c r="F15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="H15" s="56" t="s">
+      <c r="H15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="I15" s="54" t="s">
+      <c r="I15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="56" t="s">
+      <c r="J15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="K15" s="54" t="s">
+      <c r="K15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="56" t="s">
+      <c r="L15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M15" s="54" t="s">
+      <c r="M15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N15" s="56" t="s">
+      <c r="N15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O15" s="54" t="s">
+      <c r="O15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P15" s="56"/>
+      <c r="P15" s="59"/>
       <c r="Q15" s="29">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -38994,13 +39138,13 @@
       <c r="S15" s="30">
         <v>26.0</v>
       </c>
-      <c r="V15" s="31" t="s">
-        <v>171</v>
+      <c r="V15" s="63" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="26" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B16" s="37" t="s">
         <v>181</v>
@@ -39055,10 +39199,10 @@
     </row>
     <row r="17">
       <c r="A17" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="B17" s="49" t="s">
-        <v>112</v>
+        <v>227</v>
+      </c>
+      <c r="B17" s="76" t="s">
+        <v>228</v>
       </c>
       <c r="C17" s="38">
         <v>45.0</v>
@@ -39122,10 +39266,10 @@
     </row>
     <row r="20">
       <c r="A20" s="4"/>
-      <c r="D20" s="64" t="s">
+      <c r="D20" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="65">
+      <c r="E20" s="78">
         <v>15.0</v>
       </c>
       <c r="S20" s="31"/>
@@ -39140,10 +39284,10 @@
     </row>
     <row r="21">
       <c r="A21" s="4"/>
-      <c r="D21" s="64" t="s">
+      <c r="D21" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="65">
+      <c r="E21" s="78">
         <v>20.0</v>
       </c>
       <c r="S21" s="31"/>
@@ -41633,35 +41777,35 @@
     </row>
     <row r="2">
       <c r="A2" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="B2" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="54">
+      <c r="C2" s="57">
         <v>40.0</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="54">
+      <c r="E2" s="57">
         <v>20.0</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="54">
+      <c r="G2" s="57">
         <v>25.0</v>
       </c>
-      <c r="H2" s="53"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="59"/>
       <c r="Q2" s="29">
         <f t="shared" ref="Q2:Q17" si="1">SUM(C2,E2,G2,I2,K2,M2,O2)</f>
         <v>85</v>
@@ -41671,47 +41815,47 @@
       </c>
       <c r="T2" s="31"/>
       <c r="U2" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="V2" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="B3" s="53" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="57">
         <v>25.0</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="55">
+      <c r="E3" s="58">
         <v>15.0</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="54">
+      <c r="G3" s="57">
         <v>25.0</v>
       </c>
-      <c r="H3" s="53" t="s">
+      <c r="H3" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="55">
+      <c r="I3" s="58">
         <v>20.0</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="59"/>
       <c r="Q3" s="29">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -41721,10 +41865,10 @@
       </c>
       <c r="T3" s="31"/>
       <c r="U3" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="V3" s="32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4">
@@ -41761,63 +41905,63 @@
       <c r="S4" s="30">
         <v>15.0</v>
       </c>
-      <c r="T4" s="57" t="s">
+      <c r="T4" s="62" t="s">
         <v>136</v>
       </c>
       <c r="U4" s="31" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="57">
         <v>20.0</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="54">
-        <v>20.0</v>
-      </c>
-      <c r="F5" s="53" t="s">
+      <c r="E5" s="58">
+        <v>10.0</v>
+      </c>
+      <c r="F5" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="54">
+      <c r="G5" s="57">
         <v>15.0</v>
       </c>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="54">
+      <c r="I5" s="57">
         <v>10.0</v>
       </c>
-      <c r="J5" s="66" t="s">
+      <c r="J5" s="79" t="s">
         <v>98</v>
       </c>
-      <c r="K5" s="67">
+      <c r="K5" s="80">
         <v>15.0</v>
       </c>
-      <c r="L5" s="61" t="s">
+      <c r="L5" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="M5" s="59">
+      <c r="M5" s="68">
         <v>10.0</v>
       </c>
-      <c r="N5" s="56" t="s">
+      <c r="N5" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O5" s="54" t="s">
+      <c r="O5" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P5" s="56"/>
+      <c r="P5" s="59"/>
       <c r="Q5" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="S5" s="30">
         <v>16.0</v>
@@ -41825,8 +41969,8 @@
       <c r="T5" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="U5" s="68" t="s">
-        <v>209</v>
+      <c r="U5" s="81" t="s">
+        <v>231</v>
       </c>
       <c r="V5" s="31" t="s">
         <v>183</v>
@@ -41836,16 +41980,16 @@
       <c r="A6" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="70">
+      <c r="C6" s="83">
         <v>20.0</v>
       </c>
-      <c r="D6" s="69" t="s">
+      <c r="D6" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="70">
+      <c r="E6" s="83">
         <v>20.0</v>
       </c>
       <c r="F6" s="43" t="s">
@@ -41857,8 +42001,8 @@
       <c r="H6" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="I6" s="34">
-        <v>20.0</v>
+      <c r="I6" s="44">
+        <v>15.0</v>
       </c>
       <c r="J6" s="43" t="s">
         <v>66</v>
@@ -41881,14 +42025,14 @@
       <c r="P6" s="35"/>
       <c r="Q6" s="29">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="S6" s="30">
         <v>17.0</v>
       </c>
       <c r="T6" s="31"/>
       <c r="U6" s="31" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="V6" s="31" t="s">
         <v>142</v>
@@ -41898,41 +42042,41 @@
       <c r="A7" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="57">
         <v>35.0</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="54">
+      <c r="E7" s="57">
         <v>35.0</v>
       </c>
-      <c r="F7" s="58" t="s">
+      <c r="F7" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="59">
+      <c r="G7" s="68">
         <v>20.0</v>
       </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="56" t="s">
+      <c r="H7" s="75"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M7" s="54" t="s">
+      <c r="M7" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N7" s="56" t="s">
+      <c r="N7" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O7" s="54" t="s">
+      <c r="O7" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P7" s="56"/>
+      <c r="P7" s="59"/>
       <c r="Q7" s="29">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -41942,7 +42086,7 @@
       </c>
       <c r="T7" s="31"/>
       <c r="U7" s="31" t="s">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="V7" s="31" t="s">
         <v>145</v>
@@ -41973,7 +42117,7 @@
       <c r="H8" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="I8" s="60">
+      <c r="I8" s="71">
         <v>25.0</v>
       </c>
       <c r="J8" s="47" t="s">
@@ -42004,7 +42148,7 @@
       </c>
       <c r="T8" s="31"/>
       <c r="U8" s="31" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="V8" s="31" t="s">
         <v>148</v>
@@ -42014,49 +42158,49 @@
       <c r="A9" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="57">
         <v>30.0</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="57">
         <v>30.0</v>
       </c>
-      <c r="F9" s="61" t="s">
+      <c r="F9" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="59">
+      <c r="G9" s="68">
         <v>15.0</v>
       </c>
-      <c r="H9" s="56" t="s">
+      <c r="H9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="I9" s="54" t="s">
+      <c r="I9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="J9" s="56" t="s">
+      <c r="J9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="K9" s="54" t="s">
+      <c r="K9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="L9" s="56" t="s">
+      <c r="L9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M9" s="54" t="s">
+      <c r="M9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N9" s="56" t="s">
+      <c r="N9" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O9" s="54" t="s">
+      <c r="O9" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P9" s="56"/>
+      <c r="P9" s="59"/>
       <c r="Q9" s="29">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -42066,7 +42210,7 @@
       </c>
       <c r="T9" s="31"/>
       <c r="U9" s="31" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="V9" s="31" t="s">
         <v>151</v>
@@ -42076,14 +42220,14 @@
       <c r="A10" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="73" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="34">
         <v>45.0</v>
       </c>
-      <c r="D10" s="63" t="s">
-        <v>205</v>
+      <c r="D10" s="74" t="s">
+        <v>219</v>
       </c>
       <c r="E10" s="46">
         <v>25.0</v>
@@ -42140,41 +42284,41 @@
       <c r="A11" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="54">
+      <c r="C11" s="57">
         <v>10.0</v>
       </c>
-      <c r="D11" s="53" t="s">
+      <c r="D11" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="54">
+      <c r="E11" s="57">
         <v>25.0</v>
       </c>
-      <c r="F11" s="53" t="s">
+      <c r="F11" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="54">
+      <c r="G11" s="57">
         <v>20.0</v>
       </c>
-      <c r="H11" s="53" t="s">
+      <c r="H11" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="54">
+      <c r="I11" s="57">
         <v>35.0</v>
       </c>
-      <c r="J11" s="58"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="56" t="s">
+      <c r="J11" s="75"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O11" s="54" t="s">
+      <c r="O11" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P11" s="56"/>
+      <c r="P11" s="59"/>
       <c r="Q11" s="29">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -42184,7 +42328,7 @@
       </c>
       <c r="T11" s="31"/>
       <c r="U11" s="31" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="V11" s="31" t="s">
         <v>154</v>
@@ -42248,7 +42392,7 @@
         <v>162</v>
       </c>
       <c r="U12" s="31" t="s">
-        <v>215</v>
+        <v>237</v>
       </c>
       <c r="V12" s="31" t="s">
         <v>160</v>
@@ -42258,49 +42402,49 @@
       <c r="A13" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="57">
         <v>10.0</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="57">
         <v>25.0</v>
       </c>
-      <c r="F13" s="56" t="s">
+      <c r="F13" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="54">
+      <c r="G13" s="57">
         <v>25.0</v>
       </c>
-      <c r="H13" s="53" t="s">
+      <c r="H13" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="54">
+      <c r="I13" s="57">
         <v>15.0</v>
       </c>
-      <c r="J13" s="58" t="s">
+      <c r="J13" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="K13" s="59">
+      <c r="K13" s="68">
         <v>15.0</v>
       </c>
-      <c r="L13" s="56" t="s">
+      <c r="L13" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M13" s="54" t="s">
+      <c r="M13" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N13" s="56" t="s">
+      <c r="N13" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O13" s="54" t="s">
+      <c r="O13" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P13" s="56"/>
+      <c r="P13" s="59"/>
       <c r="Q13" s="29">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -42312,7 +42456,7 @@
         <v>166</v>
       </c>
       <c r="U13" s="31" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="V13" s="31" t="s">
         <v>164</v>
@@ -42370,7 +42514,7 @@
       </c>
       <c r="T14" s="31"/>
       <c r="U14" s="31" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="V14" s="31" t="s">
         <v>168</v>
@@ -42380,49 +42524,49 @@
       <c r="A15" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="54">
+      <c r="C15" s="57">
         <v>20.0</v>
       </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="54">
+      <c r="E15" s="57">
         <v>20.0</v>
       </c>
-      <c r="F15" s="56" t="s">
+      <c r="F15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="H15" s="56" t="s">
+      <c r="H15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="I15" s="54" t="s">
+      <c r="I15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="J15" s="56" t="s">
+      <c r="J15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="K15" s="54" t="s">
+      <c r="K15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="56" t="s">
+      <c r="L15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="M15" s="54" t="s">
+      <c r="M15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="N15" s="56" t="s">
+      <c r="N15" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="O15" s="54" t="s">
+      <c r="O15" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="P15" s="56"/>
+      <c r="P15" s="59"/>
       <c r="Q15" s="29">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -42431,7 +42575,7 @@
         <v>26.0</v>
       </c>
       <c r="U15" s="31" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="V15" s="31" t="s">
         <v>171</v>
@@ -42561,10 +42705,10 @@
     </row>
     <row r="20">
       <c r="A20" s="4"/>
-      <c r="D20" s="64" t="s">
+      <c r="D20" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="65">
+      <c r="E20" s="78">
         <v>15.0</v>
       </c>
       <c r="S20" s="31"/>
@@ -42579,10 +42723,10 @@
     </row>
     <row r="21">
       <c r="A21" s="4"/>
-      <c r="D21" s="64" t="s">
+      <c r="D21" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="65">
+      <c r="E21" s="78">
         <v>20.0</v>
       </c>
       <c r="S21" s="31"/>
@@ -42594,16 +42738,16 @@
     </row>
     <row r="22">
       <c r="A22" s="4"/>
-      <c r="D22" s="64" t="s">
+      <c r="D22" s="77" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="65">
+      <c r="E22" s="78">
         <v>20.0</v>
       </c>
-      <c r="H22" s="56"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="54"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="57"/>
       <c r="S22" s="31"/>
       <c r="T22" s="31"/>
       <c r="U22" s="31"/>

</xml_diff>

<commit_message>
switch enums and collections (#430)
</commit_message>
<xml_diff>
--- a/planung_pm.xlsx
+++ b/planung_pm.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="243">
   <si>
     <t>Thema</t>
   </si>
@@ -713,10 +713,13 @@
     <t>Serialisierung (equals, hashCode Wdhlg)</t>
   </si>
   <si>
+    <t>Type-Object-Pattern</t>
+  </si>
+  <si>
     <t>D4</t>
   </si>
   <si>
-    <t>K6: Serialisierung, Type Object, Flyweight, Observer</t>
+    <t>K6: Serialisierung, Type Object, Flyweight, Observer, Enumeration</t>
   </si>
   <si>
     <t>D5</t>
@@ -738,6 +741,9 @@
   </si>
   <si>
     <t>D8</t>
+  </si>
+  <si>
+    <t>K10: Multithreading</t>
   </si>
   <si>
     <t>D9</t>
@@ -1345,14 +1351,14 @@
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="9" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -38260,7 +38266,7 @@
     <col customWidth="1" min="18" max="18" width="5.71"/>
     <col customWidth="1" min="19" max="19" width="6.14"/>
     <col customWidth="1" min="20" max="20" width="13.29"/>
-    <col customWidth="1" min="21" max="22" width="44.14"/>
+    <col customWidth="1" min="21" max="22" width="32.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -38675,14 +38681,14 @@
       <c r="F8" s="70" t="s">
         <v>215</v>
       </c>
-      <c r="G8" s="46">
-        <v>20.0</v>
-      </c>
-      <c r="H8" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="I8" s="71">
-        <v>25.0</v>
+      <c r="G8" s="71">
+        <v>15.0</v>
+      </c>
+      <c r="H8" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="34">
+        <v>15.0</v>
       </c>
       <c r="J8" s="47" t="s">
         <v>43</v>
@@ -38690,22 +38696,22 @@
       <c r="K8" s="46">
         <v>10.0</v>
       </c>
-      <c r="L8" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="M8" s="46">
-        <v>10.0</v>
+      <c r="L8" s="72" t="s">
+        <v>216</v>
+      </c>
+      <c r="M8" s="71">
+        <v>15.0</v>
       </c>
       <c r="N8" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="46">
-        <v>10.0</v>
+      <c r="O8" s="71">
+        <v>15.0</v>
       </c>
       <c r="P8" s="35"/>
       <c r="Q8" s="29">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="S8" s="30">
         <v>19.0</v>
@@ -38715,7 +38721,7 @@
         <v>187</v>
       </c>
       <c r="V8" s="63" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9">
@@ -38734,7 +38740,7 @@
       <c r="E9" s="57">
         <v>30.0</v>
       </c>
-      <c r="F9" s="72" t="s">
+      <c r="F9" s="73" t="s">
         <v>38</v>
       </c>
       <c r="G9" s="68">
@@ -38774,24 +38780,24 @@
       </c>
       <c r="T9" s="31"/>
       <c r="U9" s="31" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="V9" s="63" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="74" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="34">
         <v>45.0</v>
       </c>
-      <c r="D10" s="74" t="s">
-        <v>219</v>
+      <c r="D10" s="72" t="s">
+        <v>220</v>
       </c>
       <c r="E10" s="46">
         <v>25.0</v>
@@ -38874,7 +38880,7 @@
       </c>
       <c r="J11" s="75"/>
       <c r="K11" s="68"/>
-      <c r="L11" s="72"/>
+      <c r="L11" s="73"/>
       <c r="M11" s="68"/>
       <c r="N11" s="59" t="s">
         <v>181</v>
@@ -38892,10 +38898,10 @@
       </c>
       <c r="T11" s="31"/>
       <c r="U11" s="31" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="V11" s="63" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12">
@@ -38959,7 +38965,7 @@
         <v>190</v>
       </c>
       <c r="V12" s="63" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13">
@@ -38984,11 +38990,11 @@
       <c r="G13" s="57">
         <v>25.0</v>
       </c>
-      <c r="H13" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="I13" s="57">
-        <v>15.0</v>
+      <c r="H13" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="I13" s="68">
+        <v>25.0</v>
       </c>
       <c r="J13" s="75" t="s">
         <v>89</v>
@@ -39011,7 +39017,7 @@
       <c r="P13" s="59"/>
       <c r="Q13" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="S13" s="30">
         <v>24.0</v>
@@ -39020,10 +39026,10 @@
         <v>166</v>
       </c>
       <c r="U13" s="31" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="V13" s="63" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14">
@@ -39078,10 +39084,10 @@
       </c>
       <c r="T14" s="31"/>
       <c r="U14" s="31" t="s">
-        <v>192</v>
+        <v>226</v>
       </c>
       <c r="V14" s="63" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15">
@@ -39139,7 +39145,7 @@
         <v>26.0</v>
       </c>
       <c r="V15" s="63" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16">
@@ -39199,10 +39205,10 @@
     </row>
     <row r="17">
       <c r="A17" s="26" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B17" s="76" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C17" s="38">
         <v>45.0</v>
@@ -41823,7 +41829,7 @@
     </row>
     <row r="3">
       <c r="A3" s="26" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B3" s="56" t="s">
         <v>20</v>
@@ -41909,7 +41915,7 @@
         <v>136</v>
       </c>
       <c r="U4" s="31" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5">
@@ -41946,7 +41952,7 @@
       <c r="K5" s="80">
         <v>15.0</v>
       </c>
-      <c r="L5" s="72" t="s">
+      <c r="L5" s="73" t="s">
         <v>54</v>
       </c>
       <c r="M5" s="68">
@@ -41970,7 +41976,7 @@
         <v>140</v>
       </c>
       <c r="U5" s="81" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="V5" s="31" t="s">
         <v>183</v>
@@ -42032,7 +42038,7 @@
       </c>
       <c r="T6" s="31"/>
       <c r="U6" s="31" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="V6" s="31" t="s">
         <v>142</v>
@@ -42086,7 +42092,7 @@
       </c>
       <c r="T7" s="31"/>
       <c r="U7" s="31" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="V7" s="31" t="s">
         <v>145</v>
@@ -42148,7 +42154,7 @@
       </c>
       <c r="T8" s="31"/>
       <c r="U8" s="31" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="V8" s="31" t="s">
         <v>148</v>
@@ -42170,7 +42176,7 @@
       <c r="E9" s="57">
         <v>30.0</v>
       </c>
-      <c r="F9" s="72" t="s">
+      <c r="F9" s="73" t="s">
         <v>38</v>
       </c>
       <c r="G9" s="68">
@@ -42210,7 +42216,7 @@
       </c>
       <c r="T9" s="31"/>
       <c r="U9" s="31" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="V9" s="31" t="s">
         <v>151</v>
@@ -42220,14 +42226,14 @@
       <c r="A10" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="74" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="34">
         <v>45.0</v>
       </c>
-      <c r="D10" s="74" t="s">
-        <v>219</v>
+      <c r="D10" s="72" t="s">
+        <v>220</v>
       </c>
       <c r="E10" s="46">
         <v>25.0</v>
@@ -42310,7 +42316,7 @@
       </c>
       <c r="J11" s="75"/>
       <c r="K11" s="68"/>
-      <c r="L11" s="72"/>
+      <c r="L11" s="73"/>
       <c r="M11" s="68"/>
       <c r="N11" s="59" t="s">
         <v>181</v>
@@ -42328,7 +42334,7 @@
       </c>
       <c r="T11" s="31"/>
       <c r="U11" s="31" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="V11" s="31" t="s">
         <v>154</v>
@@ -42392,7 +42398,7 @@
         <v>162</v>
       </c>
       <c r="U12" s="31" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="V12" s="31" t="s">
         <v>160</v>
@@ -42456,7 +42462,7 @@
         <v>166</v>
       </c>
       <c r="U13" s="31" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="V13" s="31" t="s">
         <v>164</v>
@@ -42514,7 +42520,7 @@
       </c>
       <c r="T14" s="31"/>
       <c r="U14" s="31" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="V14" s="31" t="s">
         <v>168</v>
@@ -42575,7 +42581,7 @@
         <v>26.0</v>
       </c>
       <c r="U15" s="31" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="V15" s="31" t="s">
         <v>171</v>

</xml_diff>

<commit_message>
Update schedule: swap enum and collections (#435)
</commit_message>
<xml_diff>
--- a/planung_pm.xlsx
+++ b/planung_pm.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="243">
   <si>
     <t>Thema</t>
   </si>
@@ -713,10 +713,13 @@
     <t>Serialisierung (equals, hashCode Wdhlg)</t>
   </si>
   <si>
+    <t>Type-Object-Pattern</t>
+  </si>
+  <si>
     <t>D4</t>
   </si>
   <si>
-    <t>K6: Serialisierung, Type Object, Flyweight, Observer</t>
+    <t>K6: Serialisierung, Type Object, Flyweight, Observer, Enumeration</t>
   </si>
   <si>
     <t>D5</t>
@@ -738,6 +741,9 @@
   </si>
   <si>
     <t>D8</t>
+  </si>
+  <si>
+    <t>K10: Multithreading</t>
   </si>
   <si>
     <t>D9</t>
@@ -1345,14 +1351,14 @@
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="9" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -38260,7 +38266,7 @@
     <col customWidth="1" min="18" max="18" width="5.71"/>
     <col customWidth="1" min="19" max="19" width="6.14"/>
     <col customWidth="1" min="20" max="20" width="13.29"/>
-    <col customWidth="1" min="21" max="22" width="44.14"/>
+    <col customWidth="1" min="21" max="22" width="32.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -38675,14 +38681,14 @@
       <c r="F8" s="70" t="s">
         <v>215</v>
       </c>
-      <c r="G8" s="46">
-        <v>20.0</v>
-      </c>
-      <c r="H8" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="I8" s="71">
-        <v>25.0</v>
+      <c r="G8" s="71">
+        <v>15.0</v>
+      </c>
+      <c r="H8" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="34">
+        <v>15.0</v>
       </c>
       <c r="J8" s="47" t="s">
         <v>43</v>
@@ -38690,22 +38696,22 @@
       <c r="K8" s="46">
         <v>10.0</v>
       </c>
-      <c r="L8" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="M8" s="46">
-        <v>10.0</v>
+      <c r="L8" s="72" t="s">
+        <v>216</v>
+      </c>
+      <c r="M8" s="71">
+        <v>15.0</v>
       </c>
       <c r="N8" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="46">
-        <v>10.0</v>
+      <c r="O8" s="71">
+        <v>15.0</v>
       </c>
       <c r="P8" s="35"/>
       <c r="Q8" s="29">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="S8" s="30">
         <v>19.0</v>
@@ -38715,7 +38721,7 @@
         <v>187</v>
       </c>
       <c r="V8" s="63" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9">
@@ -38734,7 +38740,7 @@
       <c r="E9" s="57">
         <v>30.0</v>
       </c>
-      <c r="F9" s="72" t="s">
+      <c r="F9" s="73" t="s">
         <v>38</v>
       </c>
       <c r="G9" s="68">
@@ -38774,24 +38780,24 @@
       </c>
       <c r="T9" s="31"/>
       <c r="U9" s="31" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="V9" s="63" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="74" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="34">
         <v>45.0</v>
       </c>
-      <c r="D10" s="74" t="s">
-        <v>219</v>
+      <c r="D10" s="72" t="s">
+        <v>220</v>
       </c>
       <c r="E10" s="46">
         <v>25.0</v>
@@ -38874,7 +38880,7 @@
       </c>
       <c r="J11" s="75"/>
       <c r="K11" s="68"/>
-      <c r="L11" s="72"/>
+      <c r="L11" s="73"/>
       <c r="M11" s="68"/>
       <c r="N11" s="59" t="s">
         <v>181</v>
@@ -38892,10 +38898,10 @@
       </c>
       <c r="T11" s="31"/>
       <c r="U11" s="31" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="V11" s="63" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12">
@@ -38959,7 +38965,7 @@
         <v>190</v>
       </c>
       <c r="V12" s="63" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13">
@@ -38984,11 +38990,11 @@
       <c r="G13" s="57">
         <v>25.0</v>
       </c>
-      <c r="H13" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="I13" s="57">
-        <v>15.0</v>
+      <c r="H13" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="I13" s="68">
+        <v>25.0</v>
       </c>
       <c r="J13" s="75" t="s">
         <v>89</v>
@@ -39011,7 +39017,7 @@
       <c r="P13" s="59"/>
       <c r="Q13" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="S13" s="30">
         <v>24.0</v>
@@ -39020,10 +39026,10 @@
         <v>166</v>
       </c>
       <c r="U13" s="31" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="V13" s="63" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14">
@@ -39078,10 +39084,10 @@
       </c>
       <c r="T14" s="31"/>
       <c r="U14" s="31" t="s">
-        <v>192</v>
+        <v>226</v>
       </c>
       <c r="V14" s="63" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15">
@@ -39139,7 +39145,7 @@
         <v>26.0</v>
       </c>
       <c r="V15" s="63" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16">
@@ -39199,10 +39205,10 @@
     </row>
     <row r="17">
       <c r="A17" s="26" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B17" s="76" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C17" s="38">
         <v>45.0</v>
@@ -41823,7 +41829,7 @@
     </row>
     <row r="3">
       <c r="A3" s="26" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B3" s="56" t="s">
         <v>20</v>
@@ -41909,7 +41915,7 @@
         <v>136</v>
       </c>
       <c r="U4" s="31" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5">
@@ -41946,7 +41952,7 @@
       <c r="K5" s="80">
         <v>15.0</v>
       </c>
-      <c r="L5" s="72" t="s">
+      <c r="L5" s="73" t="s">
         <v>54</v>
       </c>
       <c r="M5" s="68">
@@ -41970,7 +41976,7 @@
         <v>140</v>
       </c>
       <c r="U5" s="81" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="V5" s="31" t="s">
         <v>183</v>
@@ -42032,7 +42038,7 @@
       </c>
       <c r="T6" s="31"/>
       <c r="U6" s="31" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="V6" s="31" t="s">
         <v>142</v>
@@ -42086,7 +42092,7 @@
       </c>
       <c r="T7" s="31"/>
       <c r="U7" s="31" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="V7" s="31" t="s">
         <v>145</v>
@@ -42148,7 +42154,7 @@
       </c>
       <c r="T8" s="31"/>
       <c r="U8" s="31" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="V8" s="31" t="s">
         <v>148</v>
@@ -42170,7 +42176,7 @@
       <c r="E9" s="57">
         <v>30.0</v>
       </c>
-      <c r="F9" s="72" t="s">
+      <c r="F9" s="73" t="s">
         <v>38</v>
       </c>
       <c r="G9" s="68">
@@ -42210,7 +42216,7 @@
       </c>
       <c r="T9" s="31"/>
       <c r="U9" s="31" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="V9" s="31" t="s">
         <v>151</v>
@@ -42220,14 +42226,14 @@
       <c r="A10" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="74" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="34">
         <v>45.0</v>
       </c>
-      <c r="D10" s="74" t="s">
-        <v>219</v>
+      <c r="D10" s="72" t="s">
+        <v>220</v>
       </c>
       <c r="E10" s="46">
         <v>25.0</v>
@@ -42310,7 +42316,7 @@
       </c>
       <c r="J11" s="75"/>
       <c r="K11" s="68"/>
-      <c r="L11" s="72"/>
+      <c r="L11" s="73"/>
       <c r="M11" s="68"/>
       <c r="N11" s="59" t="s">
         <v>181</v>
@@ -42328,7 +42334,7 @@
       </c>
       <c r="T11" s="31"/>
       <c r="U11" s="31" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="V11" s="31" t="s">
         <v>154</v>
@@ -42392,7 +42398,7 @@
         <v>162</v>
       </c>
       <c r="U12" s="31" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="V12" s="31" t="s">
         <v>160</v>
@@ -42456,7 +42462,7 @@
         <v>166</v>
       </c>
       <c r="U13" s="31" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="V13" s="31" t="s">
         <v>164</v>
@@ -42514,7 +42520,7 @@
       </c>
       <c r="T14" s="31"/>
       <c r="U14" s="31" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="V14" s="31" t="s">
         <v>168</v>
@@ -42575,7 +42581,7 @@
         <v>26.0</v>
       </c>
       <c r="U15" s="31" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="V15" s="31" t="s">
         <v>171</v>

</xml_diff>

<commit_message>
final rescheduling: move collections to last week
</commit_message>
<xml_diff>
--- a/planung_pm.xlsx
+++ b/planung_pm.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="254">
   <si>
     <t>Thema</t>
   </si>
@@ -764,6 +764,12 @@
     <t>D8</t>
   </si>
   <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Build1: Ant</t>
+  </si>
+  <si>
     <t>K10: Multithreading</t>
   </si>
   <si>
@@ -840,7 +846,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -942,7 +948,7 @@
     <font>
       <b/>
       <u/>
-      <color theme="1"/>
+      <color rgb="FF6AA84F"/>
       <name val="Helvetica Neue"/>
       <scheme val="minor"/>
     </font>
@@ -976,6 +982,13 @@
       <u/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1161,7 +1174,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="91">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1393,6 +1406,9 @@
     <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="5" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1420,8 +1436,14 @@
     <xf borderId="0" fillId="4" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -38303,7 +38325,7 @@
     <col customWidth="1" min="15" max="15" width="8.14"/>
     <col customWidth="1" hidden="1" min="16" max="16" width="12.43"/>
     <col customWidth="1" hidden="1" min="17" max="17" width="8.14"/>
-    <col customWidth="1" min="18" max="18" width="5.29"/>
+    <col customWidth="1" hidden="1" min="18" max="18" width="5.29"/>
     <col hidden="1" min="19" max="19" width="14.43"/>
     <col customWidth="1" min="20" max="20" width="5.71"/>
     <col customWidth="1" min="21" max="21" width="6.14"/>
@@ -38867,7 +38889,7 @@
       <c r="B10" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="68">
         <v>45.0</v>
       </c>
       <c r="D10" s="69" t="s">
@@ -38930,36 +38952,32 @@
       <c r="A11" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="57">
-        <v>10.0</v>
-      </c>
-      <c r="D11" s="56" t="s">
+      <c r="C11" s="54">
+        <v>25.0</v>
+      </c>
+      <c r="D11" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="57">
+      <c r="E11" s="55">
         <v>25.0</v>
       </c>
-      <c r="F11" s="56" t="s">
+      <c r="F11" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="57">
-        <v>20.0</v>
-      </c>
-      <c r="H11" s="56" t="s">
+      <c r="G11" s="54">
+        <v>15.0</v>
+      </c>
+      <c r="H11" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="58">
-        <v>30.0</v>
-      </c>
-      <c r="J11" s="72" t="s">
-        <v>107</v>
-      </c>
-      <c r="K11" s="73">
-        <v>15.0</v>
-      </c>
+      <c r="I11" s="54">
+        <v>35.0</v>
+      </c>
+      <c r="J11" s="72"/>
+      <c r="K11" s="73"/>
       <c r="L11" s="74"/>
       <c r="M11" s="75"/>
       <c r="N11" s="59" t="s">
@@ -38992,42 +39010,38 @@
       <c r="A12" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="61">
+        <v>15.0</v>
+      </c>
+      <c r="D12" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="46">
-        <v>30.0</v>
-      </c>
-      <c r="D12" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="46">
+      <c r="E12" s="61">
         <v>20.0</v>
       </c>
-      <c r="F12" s="47" t="s">
+      <c r="F12" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="61">
+        <v>25.0</v>
+      </c>
+      <c r="H12" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="61">
         <v>20.0</v>
       </c>
-      <c r="H12" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="34">
-        <v>10.0</v>
-      </c>
-      <c r="J12" s="47" t="s">
+      <c r="J12" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="46">
-        <v>10.0</v>
-      </c>
-      <c r="L12" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="M12" s="34" t="s">
-        <v>181</v>
-      </c>
+      <c r="K12" s="61">
+        <v>20.0</v>
+      </c>
+      <c r="L12" s="69"/>
+      <c r="M12" s="61"/>
       <c r="N12" s="35" t="s">
         <v>181</v>
       </c>
@@ -39041,7 +39055,7 @@
       <c r="R12" s="35"/>
       <c r="S12" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="U12" s="30">
         <v>23.0</v>
@@ -39049,7 +39063,7 @@
       <c r="V12" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="W12" s="31" t="s">
+      <c r="W12" s="63" t="s">
         <v>190</v>
       </c>
       <c r="X12" s="63" t="s">
@@ -39060,42 +39074,38 @@
       <c r="A13" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="57">
-        <v>10.0</v>
-      </c>
-      <c r="D13" s="59" t="s">
+      <c r="C13" s="54">
+        <v>20.0</v>
+      </c>
+      <c r="D13" s="70" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="57">
+      <c r="E13" s="55">
         <v>25.0</v>
       </c>
-      <c r="F13" s="59" t="s">
+      <c r="F13" s="70" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="57">
-        <v>25.0</v>
-      </c>
-      <c r="H13" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="I13" s="75">
-        <v>25.0</v>
-      </c>
-      <c r="J13" s="76" t="s">
+      <c r="G13" s="54">
+        <v>15.0</v>
+      </c>
+      <c r="H13" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="K13" s="75">
+      <c r="I13" s="54">
+        <v>35.0</v>
+      </c>
+      <c r="J13" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="K13" s="55">
         <v>15.0</v>
       </c>
-      <c r="L13" s="59" t="s">
-        <v>181</v>
-      </c>
-      <c r="M13" s="57" t="s">
-        <v>181</v>
-      </c>
+      <c r="L13" s="72"/>
+      <c r="M13" s="73"/>
       <c r="N13" s="59" t="s">
         <v>181</v>
       </c>
@@ -39109,7 +39119,7 @@
       <c r="R13" s="59"/>
       <c r="S13" s="29">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="U13" s="30">
         <v>24.0</v>
@@ -39117,7 +39127,7 @@
       <c r="V13" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="W13" s="31" t="s">
+      <c r="W13" s="63" t="s">
         <v>231</v>
       </c>
       <c r="X13" s="63" t="s">
@@ -39128,29 +39138,29 @@
       <c r="A14" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="B14" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="46">
+      <c r="B14" s="69" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" s="61">
         <v>25.0</v>
       </c>
-      <c r="D14" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="34">
+      <c r="D14" s="69" t="s">
+        <v>234</v>
+      </c>
+      <c r="E14" s="61">
+        <v>25.0</v>
+      </c>
+      <c r="F14" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="68">
         <v>20.0</v>
       </c>
-      <c r="F14" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="G14" s="34">
-        <v>20.0</v>
-      </c>
-      <c r="H14" s="47" t="s">
+      <c r="H14" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="I14" s="46">
-        <v>20.0</v>
+      <c r="I14" s="61">
+        <v>35.0</v>
       </c>
       <c r="J14" s="47"/>
       <c r="K14" s="46"/>
@@ -39173,40 +39183,40 @@
       <c r="R14" s="35"/>
       <c r="S14" s="29">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="U14" s="30">
         <v>25.0</v>
       </c>
       <c r="V14" s="31"/>
-      <c r="W14" s="31" t="s">
-        <v>233</v>
+      <c r="W14" s="63" t="s">
+        <v>235</v>
       </c>
       <c r="X14" s="63" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="76" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="77">
+        <v>20.0</v>
+      </c>
+      <c r="D15" s="56" t="s">
         <v>13</v>
-      </c>
-      <c r="C15" s="57">
-        <v>20.0</v>
-      </c>
-      <c r="D15" s="56" t="s">
-        <v>14</v>
       </c>
       <c r="E15" s="57">
         <v>20.0</v>
       </c>
-      <c r="F15" s="59" t="s">
-        <v>181</v>
-      </c>
-      <c r="G15" s="57" t="s">
-        <v>181</v>
+      <c r="F15" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="57">
+        <v>20.0</v>
       </c>
       <c r="H15" s="59" t="s">
         <v>181</v>
@@ -39239,13 +39249,13 @@
       <c r="R15" s="59"/>
       <c r="S15" s="29">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="U15" s="30">
         <v>26.0</v>
       </c>
       <c r="X15" s="63" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16">
@@ -39309,10 +39319,10 @@
     </row>
     <row r="17">
       <c r="A17" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="B17" s="77" t="s">
-        <v>237</v>
+        <v>238</v>
+      </c>
+      <c r="B17" s="78" t="s">
+        <v>239</v>
       </c>
       <c r="C17" s="38">
         <v>45.0</v>
@@ -39380,10 +39390,10 @@
     </row>
     <row r="20">
       <c r="A20" s="4"/>
-      <c r="D20" s="78" t="s">
+      <c r="D20" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="79">
+      <c r="E20" s="80">
         <v>15.0</v>
       </c>
       <c r="U20" s="31"/>
@@ -39398,10 +39408,10 @@
     </row>
     <row r="21">
       <c r="A21" s="4"/>
-      <c r="D21" s="78" t="s">
+      <c r="D21" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="79">
+      <c r="E21" s="80">
         <v>20.0</v>
       </c>
       <c r="U21" s="31"/>
@@ -39413,10 +39423,10 @@
     </row>
     <row r="22">
       <c r="A22" s="4"/>
-      <c r="D22" s="80" t="s">
-        <v>238</v>
-      </c>
-      <c r="E22" s="79">
+      <c r="D22" s="81" t="s">
+        <v>240</v>
+      </c>
+      <c r="E22" s="80">
         <v>15.0</v>
       </c>
       <c r="U22" s="31"/>
@@ -41943,7 +41953,7 @@
     </row>
     <row r="3">
       <c r="A3" s="26" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B3" s="56" t="s">
         <v>20</v>
@@ -42029,7 +42039,7 @@
         <v>136</v>
       </c>
       <c r="U4" s="31" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5">
@@ -42060,10 +42070,10 @@
       <c r="I5" s="57">
         <v>10.0</v>
       </c>
-      <c r="J5" s="81" t="s">
+      <c r="J5" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="K5" s="82">
+      <c r="K5" s="83">
         <v>15.0</v>
       </c>
       <c r="L5" s="74" t="s">
@@ -42089,8 +42099,8 @@
       <c r="T5" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="U5" s="83" t="s">
-        <v>241</v>
+      <c r="U5" s="84" t="s">
+        <v>243</v>
       </c>
       <c r="V5" s="31" t="s">
         <v>183</v>
@@ -42100,16 +42110,16 @@
       <c r="A6" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="85">
+      <c r="C6" s="86">
         <v>20.0</v>
       </c>
-      <c r="D6" s="84" t="s">
+      <c r="D6" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="85">
+      <c r="E6" s="86">
         <v>20.0</v>
       </c>
       <c r="F6" s="43" t="s">
@@ -42152,7 +42162,7 @@
       </c>
       <c r="T6" s="31"/>
       <c r="U6" s="31" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="V6" s="31" t="s">
         <v>142</v>
@@ -42174,15 +42184,15 @@
       <c r="E7" s="57">
         <v>35.0</v>
       </c>
-      <c r="F7" s="76" t="s">
+      <c r="F7" s="87" t="s">
         <v>49</v>
       </c>
       <c r="G7" s="75">
         <v>20.0</v>
       </c>
-      <c r="H7" s="76"/>
+      <c r="H7" s="87"/>
       <c r="I7" s="75"/>
-      <c r="J7" s="76"/>
+      <c r="J7" s="87"/>
       <c r="K7" s="75"/>
       <c r="L7" s="59" t="s">
         <v>181</v>
@@ -42206,7 +42216,7 @@
       </c>
       <c r="T7" s="31"/>
       <c r="U7" s="31" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="V7" s="31" t="s">
         <v>145</v>
@@ -42237,7 +42247,7 @@
       <c r="H8" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="I8" s="86">
+      <c r="I8" s="88">
         <v>25.0</v>
       </c>
       <c r="J8" s="47" t="s">
@@ -42268,7 +42278,7 @@
       </c>
       <c r="T8" s="31"/>
       <c r="U8" s="31" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="V8" s="31" t="s">
         <v>148</v>
@@ -42330,7 +42340,7 @@
       </c>
       <c r="T9" s="31"/>
       <c r="U9" s="31" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="V9" s="31" t="s">
         <v>151</v>
@@ -42340,14 +42350,14 @@
       <c r="A10" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="89" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="34">
         <v>45.0</v>
       </c>
-      <c r="D10" s="87" t="s">
-        <v>246</v>
+      <c r="D10" s="90" t="s">
+        <v>248</v>
       </c>
       <c r="E10" s="46">
         <v>25.0</v>
@@ -42428,7 +42438,7 @@
       <c r="I11" s="57">
         <v>35.0</v>
       </c>
-      <c r="J11" s="76"/>
+      <c r="J11" s="87"/>
       <c r="K11" s="75"/>
       <c r="L11" s="74"/>
       <c r="M11" s="75"/>
@@ -42448,7 +42458,7 @@
       </c>
       <c r="T11" s="31"/>
       <c r="U11" s="31" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="V11" s="31" t="s">
         <v>154</v>
@@ -42512,7 +42522,7 @@
         <v>162</v>
       </c>
       <c r="U12" s="31" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="V12" s="31" t="s">
         <v>160</v>
@@ -42546,7 +42556,7 @@
       <c r="I13" s="57">
         <v>15.0</v>
       </c>
-      <c r="J13" s="76" t="s">
+      <c r="J13" s="87" t="s">
         <v>89</v>
       </c>
       <c r="K13" s="75">
@@ -42576,7 +42586,7 @@
         <v>166</v>
       </c>
       <c r="U13" s="31" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="V13" s="31" t="s">
         <v>164</v>
@@ -42634,7 +42644,7 @@
       </c>
       <c r="T14" s="31"/>
       <c r="U14" s="31" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="V14" s="31" t="s">
         <v>168</v>
@@ -42695,7 +42705,7 @@
         <v>26.0</v>
       </c>
       <c r="U15" s="31" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="V15" s="31" t="s">
         <v>171</v>
@@ -42825,10 +42835,10 @@
     </row>
     <row r="20">
       <c r="A20" s="4"/>
-      <c r="D20" s="78" t="s">
+      <c r="D20" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="79">
+      <c r="E20" s="80">
         <v>15.0</v>
       </c>
       <c r="S20" s="31"/>
@@ -42843,10 +42853,10 @@
     </row>
     <row r="21">
       <c r="A21" s="4"/>
-      <c r="D21" s="78" t="s">
+      <c r="D21" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="79">
+      <c r="E21" s="80">
         <v>20.0</v>
       </c>
       <c r="S21" s="31"/>
@@ -42858,10 +42868,10 @@
     </row>
     <row r="22">
       <c r="A22" s="4"/>
-      <c r="D22" s="78" t="s">
+      <c r="D22" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="79">
+      <c r="E22" s="80">
         <v>20.0</v>
       </c>
       <c r="H22" s="59"/>

</xml_diff>

<commit_message>
[VL] final rescheduling: move collections to last week (#542)
final rescheduling: move collections to last week
</commit_message>
<xml_diff>
--- a/planung_pm.xlsx
+++ b/planung_pm.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="254">
   <si>
     <t>Thema</t>
   </si>
@@ -764,6 +764,12 @@
     <t>D8</t>
   </si>
   <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Build1: Ant</t>
+  </si>
+  <si>
     <t>K10: Multithreading</t>
   </si>
   <si>
@@ -840,7 +846,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -942,7 +948,7 @@
     <font>
       <b/>
       <u/>
-      <color theme="1"/>
+      <color rgb="FF6AA84F"/>
       <name val="Helvetica Neue"/>
       <scheme val="minor"/>
     </font>
@@ -976,6 +982,13 @@
       <u/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1161,7 +1174,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="91">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1393,6 +1406,9 @@
     <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="5" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
@@ -1420,8 +1436,14 @@
     <xf borderId="0" fillId="4" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -38303,7 +38325,7 @@
     <col customWidth="1" min="15" max="15" width="8.14"/>
     <col customWidth="1" hidden="1" min="16" max="16" width="12.43"/>
     <col customWidth="1" hidden="1" min="17" max="17" width="8.14"/>
-    <col customWidth="1" min="18" max="18" width="5.29"/>
+    <col customWidth="1" hidden="1" min="18" max="18" width="5.29"/>
     <col hidden="1" min="19" max="19" width="14.43"/>
     <col customWidth="1" min="20" max="20" width="5.71"/>
     <col customWidth="1" min="21" max="21" width="6.14"/>
@@ -38867,7 +38889,7 @@
       <c r="B10" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="68">
         <v>45.0</v>
       </c>
       <c r="D10" s="69" t="s">
@@ -38930,36 +38952,32 @@
       <c r="A11" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="57">
-        <v>10.0</v>
-      </c>
-      <c r="D11" s="56" t="s">
+      <c r="C11" s="54">
+        <v>25.0</v>
+      </c>
+      <c r="D11" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="57">
+      <c r="E11" s="55">
         <v>25.0</v>
       </c>
-      <c r="F11" s="56" t="s">
+      <c r="F11" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="57">
-        <v>20.0</v>
-      </c>
-      <c r="H11" s="56" t="s">
+      <c r="G11" s="54">
+        <v>15.0</v>
+      </c>
+      <c r="H11" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="58">
-        <v>30.0</v>
-      </c>
-      <c r="J11" s="72" t="s">
-        <v>107</v>
-      </c>
-      <c r="K11" s="73">
-        <v>15.0</v>
-      </c>
+      <c r="I11" s="54">
+        <v>35.0</v>
+      </c>
+      <c r="J11" s="72"/>
+      <c r="K11" s="73"/>
       <c r="L11" s="74"/>
       <c r="M11" s="75"/>
       <c r="N11" s="59" t="s">
@@ -38992,42 +39010,38 @@
       <c r="A12" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="61">
+        <v>15.0</v>
+      </c>
+      <c r="D12" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="46">
-        <v>30.0</v>
-      </c>
-      <c r="D12" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="46">
+      <c r="E12" s="61">
         <v>20.0</v>
       </c>
-      <c r="F12" s="47" t="s">
+      <c r="F12" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="61">
+        <v>25.0</v>
+      </c>
+      <c r="H12" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="61">
         <v>20.0</v>
       </c>
-      <c r="H12" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="34">
-        <v>10.0</v>
-      </c>
-      <c r="J12" s="47" t="s">
+      <c r="J12" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="46">
-        <v>10.0</v>
-      </c>
-      <c r="L12" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="M12" s="34" t="s">
-        <v>181</v>
-      </c>
+      <c r="K12" s="61">
+        <v>20.0</v>
+      </c>
+      <c r="L12" s="69"/>
+      <c r="M12" s="61"/>
       <c r="N12" s="35" t="s">
         <v>181</v>
       </c>
@@ -39041,7 +39055,7 @@
       <c r="R12" s="35"/>
       <c r="S12" s="29">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="U12" s="30">
         <v>23.0</v>
@@ -39049,7 +39063,7 @@
       <c r="V12" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="W12" s="31" t="s">
+      <c r="W12" s="63" t="s">
         <v>190</v>
       </c>
       <c r="X12" s="63" t="s">
@@ -39060,42 +39074,38 @@
       <c r="A13" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="57">
-        <v>10.0</v>
-      </c>
-      <c r="D13" s="59" t="s">
+      <c r="C13" s="54">
+        <v>20.0</v>
+      </c>
+      <c r="D13" s="70" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="57">
+      <c r="E13" s="55">
         <v>25.0</v>
       </c>
-      <c r="F13" s="59" t="s">
+      <c r="F13" s="70" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="57">
-        <v>25.0</v>
-      </c>
-      <c r="H13" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="I13" s="75">
-        <v>25.0</v>
-      </c>
-      <c r="J13" s="76" t="s">
+      <c r="G13" s="54">
+        <v>15.0</v>
+      </c>
+      <c r="H13" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="K13" s="75">
+      <c r="I13" s="54">
+        <v>35.0</v>
+      </c>
+      <c r="J13" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="K13" s="55">
         <v>15.0</v>
       </c>
-      <c r="L13" s="59" t="s">
-        <v>181</v>
-      </c>
-      <c r="M13" s="57" t="s">
-        <v>181</v>
-      </c>
+      <c r="L13" s="72"/>
+      <c r="M13" s="73"/>
       <c r="N13" s="59" t="s">
         <v>181</v>
       </c>
@@ -39109,7 +39119,7 @@
       <c r="R13" s="59"/>
       <c r="S13" s="29">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="U13" s="30">
         <v>24.0</v>
@@ -39117,7 +39127,7 @@
       <c r="V13" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="W13" s="31" t="s">
+      <c r="W13" s="63" t="s">
         <v>231</v>
       </c>
       <c r="X13" s="63" t="s">
@@ -39128,29 +39138,29 @@
       <c r="A14" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="B14" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="46">
+      <c r="B14" s="69" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" s="61">
         <v>25.0</v>
       </c>
-      <c r="D14" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="34">
+      <c r="D14" s="69" t="s">
+        <v>234</v>
+      </c>
+      <c r="E14" s="61">
+        <v>25.0</v>
+      </c>
+      <c r="F14" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="68">
         <v>20.0</v>
       </c>
-      <c r="F14" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="G14" s="34">
-        <v>20.0</v>
-      </c>
-      <c r="H14" s="47" t="s">
+      <c r="H14" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="I14" s="46">
-        <v>20.0</v>
+      <c r="I14" s="61">
+        <v>35.0</v>
       </c>
       <c r="J14" s="47"/>
       <c r="K14" s="46"/>
@@ -39173,40 +39183,40 @@
       <c r="R14" s="35"/>
       <c r="S14" s="29">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="U14" s="30">
         <v>25.0</v>
       </c>
       <c r="V14" s="31"/>
-      <c r="W14" s="31" t="s">
-        <v>233</v>
+      <c r="W14" s="63" t="s">
+        <v>235</v>
       </c>
       <c r="X14" s="63" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="76" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="77">
+        <v>20.0</v>
+      </c>
+      <c r="D15" s="56" t="s">
         <v>13</v>
-      </c>
-      <c r="C15" s="57">
-        <v>20.0</v>
-      </c>
-      <c r="D15" s="56" t="s">
-        <v>14</v>
       </c>
       <c r="E15" s="57">
         <v>20.0</v>
       </c>
-      <c r="F15" s="59" t="s">
-        <v>181</v>
-      </c>
-      <c r="G15" s="57" t="s">
-        <v>181</v>
+      <c r="F15" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="57">
+        <v>20.0</v>
       </c>
       <c r="H15" s="59" t="s">
         <v>181</v>
@@ -39239,13 +39249,13 @@
       <c r="R15" s="59"/>
       <c r="S15" s="29">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="U15" s="30">
         <v>26.0</v>
       </c>
       <c r="X15" s="63" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16">
@@ -39309,10 +39319,10 @@
     </row>
     <row r="17">
       <c r="A17" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="B17" s="77" t="s">
-        <v>237</v>
+        <v>238</v>
+      </c>
+      <c r="B17" s="78" t="s">
+        <v>239</v>
       </c>
       <c r="C17" s="38">
         <v>45.0</v>
@@ -39380,10 +39390,10 @@
     </row>
     <row r="20">
       <c r="A20" s="4"/>
-      <c r="D20" s="78" t="s">
+      <c r="D20" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="79">
+      <c r="E20" s="80">
         <v>15.0</v>
       </c>
       <c r="U20" s="31"/>
@@ -39398,10 +39408,10 @@
     </row>
     <row r="21">
       <c r="A21" s="4"/>
-      <c r="D21" s="78" t="s">
+      <c r="D21" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="79">
+      <c r="E21" s="80">
         <v>20.0</v>
       </c>
       <c r="U21" s="31"/>
@@ -39413,10 +39423,10 @@
     </row>
     <row r="22">
       <c r="A22" s="4"/>
-      <c r="D22" s="80" t="s">
-        <v>238</v>
-      </c>
-      <c r="E22" s="79">
+      <c r="D22" s="81" t="s">
+        <v>240</v>
+      </c>
+      <c r="E22" s="80">
         <v>15.0</v>
       </c>
       <c r="U22" s="31"/>
@@ -41943,7 +41953,7 @@
     </row>
     <row r="3">
       <c r="A3" s="26" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B3" s="56" t="s">
         <v>20</v>
@@ -42029,7 +42039,7 @@
         <v>136</v>
       </c>
       <c r="U4" s="31" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5">
@@ -42060,10 +42070,10 @@
       <c r="I5" s="57">
         <v>10.0</v>
       </c>
-      <c r="J5" s="81" t="s">
+      <c r="J5" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="K5" s="82">
+      <c r="K5" s="83">
         <v>15.0</v>
       </c>
       <c r="L5" s="74" t="s">
@@ -42089,8 +42099,8 @@
       <c r="T5" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="U5" s="83" t="s">
-        <v>241</v>
+      <c r="U5" s="84" t="s">
+        <v>243</v>
       </c>
       <c r="V5" s="31" t="s">
         <v>183</v>
@@ -42100,16 +42110,16 @@
       <c r="A6" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="85">
+      <c r="C6" s="86">
         <v>20.0</v>
       </c>
-      <c r="D6" s="84" t="s">
+      <c r="D6" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="85">
+      <c r="E6" s="86">
         <v>20.0</v>
       </c>
       <c r="F6" s="43" t="s">
@@ -42152,7 +42162,7 @@
       </c>
       <c r="T6" s="31"/>
       <c r="U6" s="31" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="V6" s="31" t="s">
         <v>142</v>
@@ -42174,15 +42184,15 @@
       <c r="E7" s="57">
         <v>35.0</v>
       </c>
-      <c r="F7" s="76" t="s">
+      <c r="F7" s="87" t="s">
         <v>49</v>
       </c>
       <c r="G7" s="75">
         <v>20.0</v>
       </c>
-      <c r="H7" s="76"/>
+      <c r="H7" s="87"/>
       <c r="I7" s="75"/>
-      <c r="J7" s="76"/>
+      <c r="J7" s="87"/>
       <c r="K7" s="75"/>
       <c r="L7" s="59" t="s">
         <v>181</v>
@@ -42206,7 +42216,7 @@
       </c>
       <c r="T7" s="31"/>
       <c r="U7" s="31" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="V7" s="31" t="s">
         <v>145</v>
@@ -42237,7 +42247,7 @@
       <c r="H8" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="I8" s="86">
+      <c r="I8" s="88">
         <v>25.0</v>
       </c>
       <c r="J8" s="47" t="s">
@@ -42268,7 +42278,7 @@
       </c>
       <c r="T8" s="31"/>
       <c r="U8" s="31" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="V8" s="31" t="s">
         <v>148</v>
@@ -42330,7 +42340,7 @@
       </c>
       <c r="T9" s="31"/>
       <c r="U9" s="31" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="V9" s="31" t="s">
         <v>151</v>
@@ -42340,14 +42350,14 @@
       <c r="A10" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="89" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="34">
         <v>45.0</v>
       </c>
-      <c r="D10" s="87" t="s">
-        <v>246</v>
+      <c r="D10" s="90" t="s">
+        <v>248</v>
       </c>
       <c r="E10" s="46">
         <v>25.0</v>
@@ -42428,7 +42438,7 @@
       <c r="I11" s="57">
         <v>35.0</v>
       </c>
-      <c r="J11" s="76"/>
+      <c r="J11" s="87"/>
       <c r="K11" s="75"/>
       <c r="L11" s="74"/>
       <c r="M11" s="75"/>
@@ -42448,7 +42458,7 @@
       </c>
       <c r="T11" s="31"/>
       <c r="U11" s="31" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="V11" s="31" t="s">
         <v>154</v>
@@ -42512,7 +42522,7 @@
         <v>162</v>
       </c>
       <c r="U12" s="31" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="V12" s="31" t="s">
         <v>160</v>
@@ -42546,7 +42556,7 @@
       <c r="I13" s="57">
         <v>15.0</v>
       </c>
-      <c r="J13" s="76" t="s">
+      <c r="J13" s="87" t="s">
         <v>89</v>
       </c>
       <c r="K13" s="75">
@@ -42576,7 +42586,7 @@
         <v>166</v>
       </c>
       <c r="U13" s="31" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="V13" s="31" t="s">
         <v>164</v>
@@ -42634,7 +42644,7 @@
       </c>
       <c r="T14" s="31"/>
       <c r="U14" s="31" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="V14" s="31" t="s">
         <v>168</v>
@@ -42695,7 +42705,7 @@
         <v>26.0</v>
       </c>
       <c r="U15" s="31" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="V15" s="31" t="s">
         <v>171</v>
@@ -42825,10 +42835,10 @@
     </row>
     <row r="20">
       <c r="A20" s="4"/>
-      <c r="D20" s="78" t="s">
+      <c r="D20" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="79">
+      <c r="E20" s="80">
         <v>15.0</v>
       </c>
       <c r="S20" s="31"/>
@@ -42843,10 +42853,10 @@
     </row>
     <row r="21">
       <c r="A21" s="4"/>
-      <c r="D21" s="78" t="s">
+      <c r="D21" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="79">
+      <c r="E21" s="80">
         <v>20.0</v>
       </c>
       <c r="S21" s="31"/>
@@ -42858,10 +42868,10 @@
     </row>
     <row r="22">
       <c r="A22" s="4"/>
-      <c r="D22" s="78" t="s">
+      <c r="D22" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="79">
+      <c r="E22" s="80">
         <v>20.0</v>
       </c>
       <c r="H22" s="59"/>

</xml_diff>